<commit_message>
The code is faster when written in the wikipedia_test.py file, so that will probably be utilized to put all of the data on the excel sheet. Be sure to remove the counter variable's restriction on the while loop
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D7:D8"/>
@@ -462,17 +462,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Farming</t>
+          <t>Southwest Airlines Flight 1248</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Farming is growing crops or keeping animals by people for food and raw materials. Farming is a part of agriculture. </t>
+          <t>Southwest Airlines Flight 1248 was a regularly-scheduled passenger flight from Baltimore to Chicago-Midway. On approach, the aircraft skid off the runway and into a street, killing a 6 year old boy in a car. It was the first fatal accident in the company's history.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Agriculture is the science and art of cultivating plants and livestock. Agriculture was the key development in the rise of sedentary human civilization, whereby farming of domesticated species created food surpluses that enabled people to live in cities. The history of agriculture began thousands of years ago. After gathering wild grains beginning at least 105,000 years ago, nascent farmers began to plant them around 11,500 years ago. Pigs, sheep and cattle were domesticated over 10,000 years ago. Plants were independently cultivated in at least 11 regions of the world. Industrial agriculture based on large-scale monoculture in the twentieth century came to dominate agricultural output, though about 2 billion people still depended on subsistence agriculture into the twenty-first.</t>
+          <t>Southwest Airlines Flight 1248 (WN1248, SWA1248) was a scheduled passenger flight from Baltimore, Maryland, to Chicago, Illinois, to Salt Lake City, Utah, and then to Las Vegas, Nevada. On December 8, 2005, the airplane slid off a runway at Chicago-Midway while landing in a snowstorm and crashed into automobile traffic, killing a six-year-old boy.</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -482,17 +482,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Arithmetic</t>
+          <t>Norman Fowler, Baron Fowler</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Arithmetic is a name for working with numbers. It is a part of mathematics. The four basic arithmetic operations are addition, subtraction, multiplication, and division.</t>
+          <t>Peter Norman Fowler, Baron Fowler, PC (born 2 February 1938) is a British politician. He was a member of Margaret Thatcher's ministry. He is currently the Lord Speaker, having assumed office at the beginning of September 2016.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Arithmetic (from the Greek ἀριθμός arithmos, 'number' and τική [τέχνη], tiké [téchne], 'art') is a branch of mathematics that consists of the study of numbers, especially the properties of the traditional operations on them—addition, subtraction, multiplication and division. Arithmetic is an elementary part of number theory, and number theory is considered to be one of the top-level divisions of modern mathematics, along with algebra, geometry, and analysis. The terms arithmetic and higher arithmetic were used until the beginning of the 20th century as synonyms for number theory and are sometimes still used to refer to a wider part of number theory.</t>
+          <t>Peter Norman Fowler, Baron Fowler  (born 2 February 1938) is a British politician who served as a member of both Margaret Thatcher and John Major's ministries during the 1980s and 1990s. He was elected Lord Speaker in September 2016.</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -502,17 +502,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Addition</t>
+          <t>Vera Glagoleva</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Addition is a mathematical way of putting things together.</t>
+          <t>Vera Vitalievna Glagoleva (31 January 1956 – 16 August 2017) was a Russian actress. She was born in Moscow. She was known for her roles in Christmas movies or romantic comedies. Her best known roles were in Vyyti zamuzh za kapitana, Bednaya Sasha, and in Zhenshchin obizhat ne rekomenduyetsya. Glagoleva was awarded the People's Artist of Russia in 2011.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Addition (usually signified by the plus symbol +) is one of the four basic operations of arithmetic, the other three being subtraction, multiplication and division. The addition of two whole numbers results in the total amount or sum of those values combined. The example in the adjacent picture shows a combination of three apples and two apples, making a total of five apples. This observation is equivalent to the mathematical expression "3 + 2 = 5" i.e., "3 add 2 is equal to 5".</t>
+          <t>Vera Vitalievna Glagoleva (Russian: Ве́ра Вита́льевна Глаго́лева; 31 January 1956 – 16 August 2017) was a Russian actress and film director.</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -522,17 +522,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Albigensian</t>
+          <t>Andrzej Blumenfeld</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>The Cathar faith was a version of Christianity. They were usually considered Gnostics. The word 'Cathar' comes the Greek word katharos meaning 'unpolluted' (from Tobias Churton, The Gnostics) or  "the pure ones".</t>
+          <t>Andrzej Stanisław Blumenfeld (12 August 1951 – 14 August 2017) was a Polish actor and voice dubber. He was born in Zabrze, Poland. His career began in 1973. He was known for Polish-dubbing from American movies. His best known work are The Pianist, Delivery Man, and The Witcher.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Catharism (; from the Greek: καθαροί, katharoi, "the pure [ones]") was a Christian dualist or Gnostic revival movement between the 12th and 14th centuries which thrived in Southern Europe, particularly what is now northern Italy and southern France. Followers were known as Cathars, or Good Christians, and are now mainly remembered for a prolonged period of persecution by the Catholic Church, which did not recognise their belief as being Christian. Catharism appeared in Europe in the Languedoc region of France in the 11th century, when the name first appeared. The adherents were sometimes known as Albigensians, after the city Albi in southern France where the movement first took hold. The belief may have originated in the Byzantine Empire. Catharism was initially taught by ascetic leaders who set few guidelines and so some Catharist practices and beliefs varied by region and over time. The Catholic Church denounced its practices, including the consolamentum ritual by which Cathar individuals were baptised and raised to the status of "perfect".Catharism may have had its roots in the Paulician movement in Armenia and eastern Byzantine Anatolia and certainly in the Bogomils of the First Bulgarian Empire, who were influenced by the Paulicians resettled in Thrace (Philipopolis) by the Byzantines. Though the term Cathar () has been used for centuries to identify the movement, whether it identified itself with the name is debated. In Cathar texts, the terms Good Men (Bons Hommes), Good Women (Bonnes Femmes), or Good Christians (Bons Chrétiens) are the common terms of self-identification.The idea of two gods or deistic principles, one good and the other evil, was central to Cathar beliefs. This was antithetical to the monotheistic Catholic Church, whose fundamental principle was that there was only one God, who created all things visible and invisible. Cathars believed that the good God was the God of the New Testament, creator of the spiritual realm, whereas the evil God was the God of the Old Testament, creator of the physical world whom many Cathars identified as Satan. Cathars believed human spirits were the sexless spirits of angels trapped in the material realm of the evil god, destined to be reincarnated until they achieved salvation through the consolamentum, when they would return to the good god.From the beginning of his reign, Pope Innocent III attempted to end Catharism by sending missionaries and by persuading the local authorities to act against them. In 1208, Pierre de Castelnau, Innocent's papal legate, was murdered while returning to Rome after excommunicating Count Raymond VI of Toulouse, who, in his view, was too lenient with the Cathars. Pope Innocent III then abandoned the option of sending Catholic missionaries and jurists, declared Pierre de Castelnau a martyr and launched the Albigensian Crusade in 1209. The Crusade ended in 1229 with the defeat of the Cathars. Catharism underwent persecution by the Medieval Inquisition, which succeeded in eradicating it by 1350.</t>
+          <t>Andrzej Stanisław Blumenfeld (12 August 1951 in Zabrze – 14 August 2017 in Warsaw) was a Polish film, television, and voice actor who worked for SDI Media Polska.</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -542,17 +542,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Aharon Yadlin</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Australia, formally the Commonwealth of Australia, is a country and sovereign state in the southern hemisphere, located in Oceania. Its capital city is Canberra, and its largest city is Sydney.</t>
+          <t>Aharon Yadlin (Hebrew: אהרן ידלין‎; born 17 April 1926) is a former Israeli educator and politician. He was born in Ben Shemen, Mandatory Palestine.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Australia, officially the Commonwealth of Australia, is a sovereign country comprising the mainland of the Australian continent, the island of Tasmania, and numerous smaller islands. It is the largest country in Oceania and the world's sixth-largest country by total area. The population of 26 million is highly urbanised and heavily concentrated on the eastern seaboard. Australia's capital is Canberra, though its largest city is Sydney. The country's other major metropolitan areas are Melbourne, Brisbane, Perth, and Adelaide.</t>
+          <t>Aharon Yadlin (Hebrew: אהרן ידלין; born 17 April 1926) is a former Israeli educator and politician.</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -562,17 +562,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>American English</t>
+          <t>Eugenio Polgovsky</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>American English or United States English is the dialect of the English language spoken in the United States of America.  It is different in some ways from other types of English, such as British English.  Many types of American English came from local dialects in England.</t>
+          <t>Eugenio Polgovsky (June 29, 1977 – August 11, 2017) was a Mexican movie director, cinematographer and editor. He was born in Mexico City, Mexico. Polgovsky was known for the Mexican documentaries "Tropic of Cancer" ( Semaine de la Critique 2005) and  Los Herederos "The Inheritors" (Mostra of Venice, Orrizontti 2008 &amp; Berlinale Generation 2009).</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>American English (AmE, AE, AmEng, USEng, en-US), sometimes called United States English or U.S. English, is the set of varieties of the English language native to the United States. Currently, American English is the most influential form of English worldwide.English is the most widely spoken language in the United States and is the de facto common language used by the federal and state governments, to the extent that all laws and compulsory education presume English as the primary language. English is explicitly given official status by 32 of the 50 state governments. While the local courts in some divisions of the United States grant equivalent status to both English and another language—for example, English and Spanish in Puerto Rico—under federal law, English is still the official language for any matters being referred to the United States district court for the territory.The use of English in the United States is a result of British colonization of the Americas. The first wave of English-speaking settlers arrived in North America during the 17th century, followed by further migrations in the 18th and 19th centuries. During the 17th century, dialects from many different regions of England existed in every American colony, allowing a process of extensive dialect mixture and leveling in which English varieties across the colonies became more homogeneous compared with varieties in England. English thus predominated in the colonies even by the end of the 17th century's first massive immigration of non-English speakers from Europe and Africa, and firsthand descriptions of a fairly uniform American English became common after the mid-18th century. Since then, American English has developed into some new varieties, including regional dialects that, in some cases, show minor influences in the last two centuries from successive waves of immigrant speakers of diverse languages, primarily European languages.American English varieties include many patterns of pronunciation, vocabulary, grammar, and particularly spelling that are unified nationwide but distinct from other English dialects around the world. Any American or Canadian accent perceived as free of noticeably local, ethnic, or cultural markers is popularly called "General" or "Standard" American, a fairly uniform accent continuum native to certain regions of the U.S. and associated nationally with broadcast mass media and highly educated speech. However, historical and present linguistic evidence does not support the notion of there being one single "mainstream" American accent. The sound of American English continues to evolve, with some local accents disappearing, but several larger regional accents having emerged in the 20th century.</t>
+          <t>Eugenio Polgovsky (Mexico City, June 29, 1977 – London, August 11th, 2017) was a Mexican filmmaker and visual artist. He worked as director, cinematographer, editor, sound designer and producer of his films. Polgovsky was known for the Mexican documentaries "Tropic of Cancer" ( Semaine de la Critique 2005) and  Los Herederos "The Inheritors" (Mostra of Venice, Orrizontti 2008 &amp; Berlinale Generation 2009).</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -582,17 +582,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Aquaculture</t>
+          <t>Vern Ehlers</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aquaculture is the farming of fish, shrimp, abalones, algae, and other seafood.  Aquaculture supplies fish, such as catfish, salmon, and trout.  It was developed a few thousand years ago in China.  Aquaculture supplies over 20% of all the seafood harvested. </t>
+          <t>Vernon James "Vern" Ehlers (February 6, 1934 – August 15, 2017) was the former U.S. Representative for Michigan's 3rd congressional district, having served from 1993 until 2011. He was a member of the Republican Party.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Aquaculture (less commonly spelled aquiculture), also known as aquafarming, is the farming of fish, crustaceans, molluscs, aquatic plants, algae, and other organisms. Aquaculture involves cultivating freshwater and saltwater populations under controlled conditions, and can be contrasted with commercial fishing, which is the harvesting of wild fish.  Mariculture refers to aquaculture practiced in marine environments and in underwater habitats.</t>
+          <t>Vernon James Ehlers (February 6, 1934 – August 15, 2017) was an American physicist and politician who represented Michigan in the U.S. House of Representatives from 1993 until his retirement in 2011. A Republican, he also served eight years in the Michigan Senate and two in the Michigan House of Representatives.</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -602,17 +602,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Abbreviation</t>
+          <t>Marie-Josephine Gaudette</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>An abbreviation is a shorter way to write a word or phrase. People use abbreviations for words that they write a lot. The English language occasionally uses the apostrophe mark ' to show that a word is written in a shorter way, but some abbreviations do not use this mark. More often, they use periods, especially the ones that come from the Latin language. Common Latin abbreviations include i.e. [id est] that is, e.g. [exempli gratia] for example, and et al. [et alia] and others.</t>
+          <t xml:space="preserve">Marie-Josephine Clarice Gaudette (25 March 1902 – 13 July 2017) was an American-born Italian supercentenarian. She was the oldest living person in Italy from the death of Emma Morano, who was the oldest living person in the world and the oldest Italian person ever on 15 April 2017 until her own death three months later. </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>An abbreviation (from Latin brevis, meaning short ) is a shortened form of a word or phrase, by any method. It may consist of a group of letters, or words taken from the full version of the word or phrase; for example, the word abbreviation can itself be represented by the abbreviation abbr., abbrv., or abbrev.; NBM, for nil (or nothing) by mouth is an abbreviated medical instruction. It may also consist of initials only, a mixture of initials and words, or words or letters representing words in another language (for example, e.g., i.e. or RSVP). Some types of abbreviations are acronyms (which are pronounceable), initialisms (using initials only), or grammatical contractions or crasis.</t>
+          <t>Italian supercentenarians are citizens, residents or emigrants from Italy who have attained or surpassed 110 years of age. As of January 2015, the Gerontology Research Group (GRG) had validated the longevity claims of 151 Italian supercentenarians. There are currently 12 known Italians alive over age 110; the oldest as of 26 June 2020 is Maria Oliva, born 16 April 1909, aged, 111 years, 71 days. The oldest Italian ever was Emma Morano, who was also the last person in the world to have been born before the year 1900. She died on 15 April 2017, aged 117 years and 137 days.</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -622,17 +622,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Angel</t>
+          <t>Sam Smith (singer)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>In many mythologies and religions, an angel is a good spirit. The word angel comes from the Greek word angelos which means "messenger". Angels appear frequently in the Old Testament, the New Testament, Qur'an and Aqdas.</t>
+          <t xml:space="preserve">Samuel Frederick "Sam" Smith (born 19 May 1992) is a British singer-songwriter. They became famous in October 2012 when the song "Latch" by Disclosure came out. In 2013, they released the single "Lay Me Down". In 2014 Smith had a single, "Stay with Me" and "Money on My Mind" through their album In the Lonely Hour, which became a major international success. </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>An angel is a supernatural being in various religions and mythologies.  Abrahamic religions often depict them as benevolent celestial intermediaries between God (or Heaven) and humanity. Other roles include protectors and guides for humans, and servants of God. Abrahamic religions describe angelic hierarchies, which vary by sect and religion. Some angels have specific names (such as Gabriel or Michael) or titles (such as seraph or archangel). Humans have also used "angel" to describe various spirits and figures in other religious traditions. The theological study of angels is known as "angelology". Those expelled from Heaven are called fallen angels, distinct from the heavenly host.</t>
+          <t>Samuel Frederick Smith (born 19 May 1992) is an English singer and songwriter. They rose to prominence in October 2012 after being featured on Disclosure's breakthrough single "Latch", which peaked at number eleven on the UK Singles Chart. Smith was subsequently featured on Naughty Boy's "La La La", which became a number one single in May 2013. In December 2013, they were nominated for the 2014 Brit Critics' Choice Award and the BBC's Sound of 2014 poll, winning both.Smith's debut studio album, In the Lonely Hour, was released in May 2014 on Capitol Records UK. The album's lead single, "Lay Me Down", was released prior to "La La La". The album's second single, "Money on My Mind", became Smith's second number one single in the UK. The third single, "Stay with Me", was an international success, reaching number one in the UK and number two on the US Billboard Hot 100, while their singles "I'm Not the Only One" and "Like I Can" reached the top ten in the UK. The album won four awards, at the 57th Annual Grammy Awards, including Best Pop Vocal Album, Best New Artist, Record of the Year, Song of the Year, and nominations for Album of the Year and Best Pop Solo Performance.</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -642,17 +642,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ad hominem</t>
+          <t>Hans Streuli</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ad hominem is a Latin word for a type of argument. It is a word often used in rhetoric. Rhetoric is the science of speaking well, and convincing other people of your ideas.</t>
+          <t>Hans Streuli (13 July 1892 – 23 May 1970) was a Swiss politician.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ad hominem (Latin for 'to the person'), short for argumentum ad hominem, is a term that refers to several types of arguments, most of which are fallacious. Typically this term refers to a rhetorical strategy where the speaker attacks the character, motive, or some other attribute of the person making an argument rather than attacking the substance of the argument itself. This avoids genuine debate by creating a diversion to some irrelevant but often highly charged issue.The most common form of this fallacy is "A makes a claim a, B asserts that A holds a property that is unwelcome, and hence B concludes that argument a is wrong".</t>
+          <t>Hans Streuli (13 July 1892 – 23 May 1970) was a Swiss politician.</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -662,17 +662,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Native American</t>
+          <t>Orthodox Jew</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Native Americans (also called Aboriginal Americans, American Indians, Amerindians or indigenous peoples of America) are the people and their descendants, who were in the Americas when Europeans arrived.  There are many different tribes of Native American people, with many different languages.  There are more than three million Native Americans in Canada and the U.S. combined.  About 51 million Native Americans live in Latin America.</t>
+          <t xml:space="preserve">Orthodox Judaism is the more traditional form of nowadays Judaism. It holds that both the scripture of the Torah and mouth-to-mouth traditions later written down in the Talmud etc., were actually and literally given by God, and that past rabbis handed them over without change and were always faithful in deciding how they applied to reality. Because of this, Orthodox Judaism is very careful in holding to the tradition of past rabbis, and is very conservative on how current rabbis may decide what the law is in new cases. Orthodox Jews consider themselves as the only truly faithful Jews and reject all the new non-Orthodox forms of Jewish thought, religious or secular, that came to be in the last 250 years (since the Jewish community lost its powers to enforce people, and Jews began to be citizens of the modern state). Even so, they are a product of new times just like everyone else: Their community organizations were created so they could separate from other Jews because those stopped being religious. The Orthodox also had to make very new ways of thinking and acting to deal with the big changes.   </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Native Americans may refer to:</t>
+          <t>Orthodox Judaism is a collective term for the traditionalist branches of contemporary Rabbinic Judaism. Theologically, it is chiefly defined by regarding the Torah, both Written and Oral, as literally revealed by God on Mount Sinai and faithfully transmitted ever since.</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -682,17 +682,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Fritz Honegger</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">The apple tree (Malus domestica) is a tree that grows fruit (such as apples) in the rose family best known for its juicy, tasty fruit. It is grown worldwide as a fruit tree. It is considered to be a low-cost fruit harvestable all over the world. </t>
+          <t>Fritz Honegger (25 July 1917 – 4 March 1999) was a Swiss politician.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>An apple is an edible fruit produced by an apple tree (Malus domestica). Apple trees are cultivated worldwide and are the most widely grown species in the genus Malus. The tree originated in Central Asia, where its wild ancestor, Malus sieversii, is still found today. Apples have been grown for thousands of years in Asia and Europe and were brought to North America by European colonists. Apples have religious and mythological significance in many cultures, including Norse, Greek and European Christian tradition.</t>
+          <t>Fritz Honegger (25 July 1917 – 4 March 1999) was a Swiss politician.</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -702,17 +702,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Abrahamic religion</t>
+          <t>Fuldera</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>An Abrahamic religion is a religion whose followers believe in the prophet Abraham and his sons/grandsons to hold an important role in human spiritual development. The best known Abrahamic religions are Judaism, Christianity and Islam. Smaller religious traditions sometimes included as Abrahamic religions are Samaritanism, Druze, Rastafari, Yazidi, Babism, Bahá'í Faith. Mandaeism, a religion holding many Abrahamic beliefs, isn’t categorized as one due to them believing Abraham was a false prophet</t>
+          <t>Fuldera is a village and former municipality of the district of Inn in the canton of Graubünden in Switzerland.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>The Abrahamic religions, also referred to collectively as Abrahamism, are a group of Semitic-originated religious communities of faith that claim descent from the Judaism of the ancient Israelites and the worship of the God of Abraham. The Abrahamic religions are monotheistic, with the term deriving from the patriarch Abraham (a major biblical figure from the Old Testament, who is recognized by Jews, Christians, Muslims, and others).Abrahamic religions spread globally through Christianity being adopted by the Roman Empire in the 4th century and Islam by the Islamic empires from the 7th century. Today the Abrahamic religions are one of the major divisions in comparative religion (along with Indian, Iranian, and East Asian religions). The major Abrahamic religions in chronological order of founding are Judaism (the base of the other two religions) in the 7th century BCE, Christianity in the 1st century CE, and Islam in the 7th century CE.</t>
+          <t>Fuldera is a village in the Val Müstair municipality in the district of Inn in the Swiss canton of Graubünden.  In 2009 Fuldera merged with Lü, Müstair, Santa Maria Val Müstair, Tschierv and Valchava to form the municipality of Val Müstair.</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -722,17 +722,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Algebra</t>
+          <t>Fadwa Soliman</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Algebra (from Arabic: الجبر‎, transliterated "al-jabr", meaning "reunion of broken parts") is a part of mathematics (often called math in the United States and maths or numeracy in the United Kingdom ). It uses variables to represent a value that is not yet known.  When an equals sign (=) is used, this is called an equation.  A very simple equation using a variable is: 2 + 3 = x. In this example, x = 5, or it could also be said that "x equals five".  This is called solving for x.  Besides equations, there are inequalities (less than and greater than). A special type of equation is called the function.  This is often used in making graphs because it always turns one input into one output.</t>
+          <t>Fadwa Soliman or Fadwa Suleiman (17 May 1970 – 17 August 2017) was a Syrian actress and activist. She was born in Aleppo, Syria. She led a Sunni-majority protest against Bashar al-Assad's government in Homs. She became one of the most recognized faces of the Syrian Civil War.On 17 August 2017 Soliman died of cancer while in exile in Paris, aged 47.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Algebra (from Arabic: الجبر‎ (al-jabr, meaning "reunion of broken parts" and "bonesetting") is one of the broad parts of mathematics, together with number theory, geometry and analysis. In its most general form, algebra is the study of mathematical symbols and the rules for manipulating these symbols; it is a unifying thread of almost all of mathematics. It includes everything from elementary equation solving to the study of abstractions such as groups, rings, and fields. The more basic parts of algebra are called elementary algebra; the more abstract parts are called abstract algebra or modern algebra. Elementary algebra is generally considered to be essential for any study of mathematics, science, or engineering, as well as such applications as medicine and economics. Abstract algebra is a major area in advanced mathematics, studied primarily by professional mathematicians.</t>
+          <t>Fadwa Souleimane (also transcribed as Fadwa Soliman or Fadwa Suleiman; 17 May 1970 – 17 August 2017) was a Syrian actress of Alawite descent who led a Sunni-majority protest against Bashar al-Assad's government in Homs. She became one of the most recognized faces of the Syrian Civil War.</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -742,17 +742,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>As</t>
+          <t>2017 Barcelona attack</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AS or as may refer to:</t>
+          <t>On 17 August 2017, a white van hit pedestrians on La Rambla, Barcelona, leaving fourteen people dead and dozens injured. The two suspects then fled on foot.At around 17:20 CEST, a white Fiat Talento drove onto the pavement of Barcelona's Las Ramblas, crashing into pedestrians between Plaça Catalunya and Gran Teatre del Liceu.In the press conference held by the police at 7:00pm local time, the spokesperson confirmed the terrorist nature of the event, a dead person and 32 injured —10 of those in serious condition.  Other sources are claiming the fatality count is 13.Police said two men were arrested in connection with the attack; another was reported killed in a shootout with police. In Ripoll, a man in his 20s was alleged to have rented the van, but told police his ID was stolen. Amaq News Agency said the attackers were "soldiers of the Islamic State" who "carried out the operation in response to calls for targeting coalition states".An explosion happened the night before the attack in the Catalan town of Alcanar. It flattened a building and killed a woman. The head of the Mossos d'Esquadra Josep Lluís Trapero said it was related to the ramming. Nine hours after the attack, police killed four people in Tarragona said to be planning a terrorist attack in Cambrils.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>As, AS, A/S or similar may refer to:</t>
+          <t>On the afternoon of 17 August 2017, 22-year-old Younes Abouyaaqoub drove a van into pedestrians on La Rambla in Barcelona, Catalonia, Spain killing 13 people and injuring at least 130 others, one of whom died 10 days later on 27 August. Abouyaaqoub fled the attack on foot, then killed another person in order to steal the victim's car to make his escape.Nine hours after the Barcelona attack, five men thought to be members of the same terrorist cell drove into pedestrians in nearby Cambrils, killing one woman and injuring six others. All five of those attackers were shot and killed by police.The night before the Barcelona attack, an explosion occurred in a house in the Spanish town of Alcanar, destroying the building and killing two members of the terrorist cell, including the 40-year-old imam thought to be the mastermind. The home had more than 120 gas canisters inside which police believe the cell was attempting to make into one large bomb (or three smaller bombs to be placed in three vans which they had rented) but which they accidentally detonated.The Prime Minister of Spain, Mariano Rajoy, called the attack in Barcelona a jihadist attack. Amaq News Agency attributed indirect responsibility for the attack to the Islamic State of Iraq and the Levant (ISIL). The attacks were the deadliest in Spain since the March 2004 Madrid train bombings and the deadliest in Barcelona since the 1987 Hipercor bombing. Younes Abouyaaqoub, the driver of the van in the Barcelona attack, was killed by police in a town 30 miles west of Barcelona on 21 August.</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -762,17 +762,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Atom</t>
+          <t>Grentzingen</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>The atom is the basic unit of matter. It is the smallest thing that can have a chemical property.  There are many different types of atoms, each with its own name, atomic mass and size.  These different atoms are called chemical elements.  The chemical elements are organized on the periodic table.  Examples of elements are hydrogen and gold.</t>
+          <t>Grentzingen is a former commune. It is found in the Haut-Rhin department of eastern France. On 1 January 2016, it was merged into the new commune of Illtal.It is 25 km west of Basel and 10 km southeast of Altkirch.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>An atom is the smallest constituent unit of ordinary matter that constitutes a chemical element. Every solid, liquid, gas, and plasma is composed of neutral or ionized atoms. Atoms are extremely small, typically around 100 picometers across. They are so small that accurately predicting their behavior using classical physics – as if they were billiard balls, for example – is not possible due to quantum effects. Current atomic models use quantum principles to better explain and predict this behavior.</t>
+          <t>Grentzingen (German: Grenzingen) is a former commune in the Haut-Rhin department in north-eastern France. On 1 January 2016, it was merged into the new commune Illtal.</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -782,17 +782,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Astronomy</t>
+          <t>Griesbach-au-Val</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Astronomy (from the Greek astron (ἄστρον) meaning "star" and nomos (nόμος) meaning "law") is the scientific study of celestial bodies such as stars, planets, comets, and galaxies</t>
+          <t>Griesbach-au-Val is a commune. It is found in the Haut-Rhin department of eastern France.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Astronomy (from Greek: ἀστρονομία) is a natural science that studies celestial objects and phenomena. It uses mathematics, physics, and chemistry in order to explain their origin and evolution. Objects of interest include planets, moons, stars, nebulae, galaxies, and comets. Relevant phenomena include supernova explosions, gamma ray bursts, quasars, blazars, pulsars, and cosmic microwave background radiation. More generally, astronomy studies everything that originates outside Earth's atmosphere. Cosmology is a branch of astronomy. It studies the Universe as a whole.Astronomy is one of the oldest natural sciences. The early civilizations in recorded history made methodical observations of the night sky. These include the Babylonians, Greeks, Indians, Egyptians, Chinese, Maya, and many ancient indigenous peoples of the Americas. In the past, astronomy included disciplines as diverse as astrometry, celestial navigation, observational astronomy, and the making of calendars. Nowadays, professional astronomy is often said to be the same as astrophysics.Professional astronomy is split into observational and theoretical branches. Observational astronomy is focused on acquiring data from observations of astronomical objects. This data is then analyzed using basic principles of physics. Theoretical astronomy is oriented toward the development of computer or analytical models to describe astronomical objects and phenomena. These two fields complement each other. Theoretical astronomy seeks to explain observational results and observations are used to confirm theoretical results.</t>
+          <t>Griesbach-au-Val (German: Griesbach im Thal) is a commune in the Haut-Rhin department in Grand Est in north-eastern France.</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -802,17 +802,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Architecture</t>
+          <t>Grussenheim</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Architecture is the art and science of the design of structures or buildings such as houses, places of worship, and office buildings. Architecture is also the profession of an architect. Usually, a person must study at an institution of higher education (university) to become an architect. In ancient times, there were architects long before there was higher education. </t>
+          <t>Grussenheim is a commune. It is found in the Haut-Rhin department of eastern France.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Architecture (Latin architectura, from the Greek ἀρχιτέκτων arkhitekton "architect", from ἀρχι- "chief" and τέκτων "creator") is both the process and the product of planning, designing, and constructing buildings or other structures. Architectural works, in the material form of buildings, are often perceived as cultural symbols and as works of art. Historical civilizations are often identified with their surviving architectural achievements.</t>
+          <t>Grussenheim (German: Grüssenheim) is a commune in the Haut-Rhin department in Grand Est in north-eastern France.</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -822,17 +822,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Anatomy</t>
+          <t>Viaur</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Anatomy is the study of the bodies of people and other animals. Anatomy is the study of the inside of the body and outside the body. Anatomy notes the position and structure of organs such as muscles, glands and bones. A person who studies anatomy is an anatomist. </t>
+          <t>The Viaur is a river in southern France, left tributary of the Aveyron river. It flows through the Aveyron, Tarn and Tarn-et-Garonne departments.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Anatomy (Greek anatomē, 'dissection') is the branch of biology concerned with the study of the structure of organisms and their parts. Anatomy is a branch of natural science which deals with the structural organization of living things. It is an old science, having its beginnings in prehistoric times. Anatomy is inherently tied to developmental biology, embryology, comparative anatomy, evolutionary biology, and phylogeny, as these are the processes by which anatomy is generated, both over immediate and long-term timescales. Anatomy and physiology, which study the structure and function of organisms and their parts respectively, make a natural pair of related disciplines, and are often studied together. Human anatomy is one of the essential basic sciences that are applied in medicine.The discipline of anatomy is divided into macroscopic and microscopic. Macroscopic anatomy, or gross anatomy, is the examination of an animal's body parts using unaided eyesight. Gross anatomy also includes the branch of superficial anatomy. Microscopic anatomy involves the use of optical instruments in the study of the tissues of various structures, known as histology, and also in the study of cells.</t>
+          <t>The Viaur is a 168 km (104 mi) long river in south-western France. It is a left tributary of the Aveyron. Its source is in the southern Massif Central, north of Millau. It flows generally west through the following departments and towns:</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -842,17 +842,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Asteroid</t>
+          <t>M. T. Liggett</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>An asteroid is a space rock. It is a small object in the Solar System that travels around the Sun. It is like a planet but smaller. They range from very small (smaller than a car) to 600 miles (1000 km) across. A few asteroids have asteroid moon.</t>
+          <t xml:space="preserve">Myron Thomas "M. T." Liggett (December 28, 1930 – August 17, 2017) was an American folk sculptor. He was born near Mullinville, Kansas. He exhibited hundreds of his artworks on the roads of Mullinville. </t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Asteroids are minor planets, especially of the inner Solar System. Larger asteroids have also been called planetoids. These terms have historically been applied to any astronomical object orbiting the Sun that did not resolve into a disc in a telescope and was not observed to have characteristics of an active comet such as a tail. As minor planets in the outer Solar System were discovered that were found to have volatile-rich surfaces similar to comets, these came to be distinguished from the objects found in the main asteroid belt. In this article, the term "asteroid" refers to the minor planets of the inner Solar System, including those co-orbital with Jupiter.</t>
+          <t>Myron Thomas Liggett (December 28, 1930 – August 17, 2017) was an American folk sculptor.Liggett was born in Mullinville, Kansas and grew up on his family farm. He graduated from Mullinville High School. Liggett went to Dodge City Community College. He also went to the University of Texas where he majored in political science. Liggett served in the United States Navy in 1948 and then joined the United States Air Force in 1957. In 1987, Liggett returned to Mullinville, Kansas where he exhibited his art work containing re-used farm implements, welded metal and combined discs. His works were kinetic and moved with the wind. He received his bachelor's degree from Fort Hays State University and went to the University of Nevada, Las Vegas law school.M. T. Liggett's main venue was the land along his front fence, on the north side of U.S. Route 400 in Mullinville. He was also a featured artist at the Folk Art Museum in Lucas, Kansas.He and some of his sculptures appear in the 2009 documentary What's the Matter with Kansas?.Liggett died on August 17, 2017 at the age of 86 at Wesley Medical Center in Wichita, Kansas.</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -862,17 +862,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>John Boorman</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Afghanistan (officially called Islamic Republic of Afghanistan; Persian: جمهوری اسلامی افغانستان‎, Pashto: د افغانستان اسلامي جمهوريت‎) is a country located in Central Asia and South Asia. It has borders with Pakistan in the south and east, Iran in the west, Turkmenistan, Uzbekistan and Tajikistan in the north, and China in the far northeast.In early times people passed through it with animals and other goods as it connected China and India with Central Asia and the Middle East. More recently, Afghanistan has been damaged by many years of war. This has resulted in there not being enough jobs.</t>
+          <t xml:space="preserve">John Boorman (; born 18 January 1933) is an English filmmaker.Boorman is best known for his feature movies such as Point Blank, Hell in the Pacific, Leo the Last, Deliverance, Zardoz, Excalibur, The Emerald Forest, Hope and Glory, The General, The Tailor of Panama, and Queen and Country. </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Afghanistan ( (listen); Pashto/Dari: افغانستان, Pashto: Afġānistān [avɣɒnisˈtɒn, ab-], Dari: Afġānestān [avɣɒnesˈtɒn]), officially the Islamic Republic of Afghanistan, is a landlocked country in Central and South Asia. Afghanistan is bordered by Pakistan to the east and south; Iran to the west; Turkmenistan, Uzbekistan, and Tajikistan to the north; and China to the northeast. Occupying 652,000 square kilometers (252,000 sq mi), it is a mountainous country with plains in the north and southwest. Kabul is the capital and largest city. The population is around 32 million, mostly composed of ethnic Pashtuns, Tajiks, Hazaras and Uzbeks.</t>
+          <t>John Boorman ,  (born 18 January 1933) is an English filmmaker who is best known for his feature films such as Point Blank, Hell in the Pacific, Deliverance, Zardoz, Exorcist II: The Heretic, Excalibur, The Emerald Forest, Hope and Glory, The General, The Tailor of Panama and Queen and Country.</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -882,17 +882,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Angola</t>
+          <t>George Edward Glass</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Angola, (), officially the Republic of Angola, is a country in southern Africa bordered by Namibia on the south, the Democratic Republic of the Congo on the north, and Zambia on the east; its west coast is on the Atlantic Ocean with Luanda as its capital city.</t>
+          <t>George Edward Glass is an American businessman and diplomat. He has been confirmed by the United States Senate as the next United States Ambassador to Portugal. This nomination was confirmed by the U.S. Senate on August 3, 2017. He took office on August 25, 2017.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Angola ( (listen); Portuguese: [ɐ̃ˈɡɔlɐ]), officially the Republic of Angola (Portuguese: República de Angola), is a country on the west coast of Southern Africa. It is the seventh-largest country in Africa, bordered by Namibia to the south, the Democratic Republic of the Congo to the north, Zambia to the east, and the Atlantic Ocean to the west. Angola has an exclave province, the province of Cabinda that borders the Republic of the Congo and the Democratic Republic of the Congo. The capital and largest city of Angola is Luanda.</t>
+          <t>George Edward Glass (born August 27, 1960) is an American businessman and diplomat.  He currently serves as the Ambassador of the United States to the Republic of Portugal.</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -902,17 +902,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Duke Buchan</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Argentina (officially the Argentine Republic)  is a country in South America. Argentina is the second-largest country in South America and the eighth-largest country in the world.</t>
+          <t>Richard Duke Buchan III (born July 3, 1963) is an American entrepreneur, financier, farmer, and philanthropist. He is the founder and CEO of Hunter Global Investors, a private investment management firm.Buchan has been nominated by President Donald Trump to become United States Ambassador to Spain and Andorra. This nomination was confirmed by the United States Senate on November 2, 2017.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Argentina (Spanish: [aɾxenˈtina]), officially the Argentine Republic (Spanish: República Argentina), is a country located mostly in the southern half of South America. Sharing the bulk of the Southern Cone with Chile to the west, the country is also bordered by Bolivia and Paraguay to the north, Brazil to the northeast, Uruguay and the South Atlantic Ocean to the east, and the Drake Passage to the south. With a mainland area of 2,780,400 km2 (1,073,500 sq mi), Argentina is the eighth-largest country in the world, the fourth largest in the Americas, the second largest in South America after Brazil, and the largest Spanish-speaking nation. The sovereign state is subdivided into twenty-three provinces (Spanish: provincias, singular provincia) and one autonomous city (ciudad autónoma), Buenos Aires, which is the federal capital of the nation (Spanish: Capital Federal) as decided by Congress. The provinces and the capital have their own constitutions, but exist under a federal system. Argentina claims sovereignty over part of Antarctica, the Falkland Islands (Spanish: Islas Malvinas), and South Georgia and the South Sandwich Islands.</t>
+          <t>Richard Duke Buchan III (born July 3, 1963) is the United States Ambassador to Spain and Andorra. On November 2, 2017 Buchan was confirmed by the United States Senate by voice vote. He was sworn in by Vice President Mike Pence on December 11, 2017. Buchan is an American entrepreneur, financier, farmer, and philanthropist. He is the founder and CEO of Hunter Global Investors, a private investment management firm.</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -922,17 +922,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Pete Hoekstra</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Austria (German: Österreich; officially called Republic of Austria), is a country in Central Europe. Around Austria there are the countries of Germany, Czech Republic, Slovakia, Hungary, Slovenia, Italy, Switzerland, and Liechtenstein. Currently, the chancellor is Sebastian Kurz. The previous chancellor was Brigitte Bierlein (2019). Austria has been a member-state of the United Nations since 1955 the European Union since 1995 and OPEC since 2019.</t>
+          <t>Pieter "Pete" Hoekstra (; born October 30, 1953) is an American politician of Dutch descent. He is the United States Ambassador to the Netherlands since November 2017. He is a former member of the United States House of Representatives, representing Michigan's 2nd congressional district from 1993 to 2011. Hoekstra is a member of the Republican Party.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Austria ( (listen), ; German: Österreich [ˈøːstɐʁaɪ̯ç] (listen)), officially the Republic of Austria (German: Republik Österreich, listen ), is a landlocked East Alpine country in the southern part of Central Europe. It is composed of nine federated states (Bundesländer), one of which is Vienna, Austria's capital and its largest city. It is bordered by Germany to the northwest, Czech Republic to the north, Slovakia to the northeast, Hungary to the east, Slovenia and Italy to the south, and Switzerland and Liechtenstein to the west. Austria occupies an area of 83,879 km2 (32,386 sq mi) and has a population of nearly 9 million people. While German is the country's official language, many Austrians communicate informally in a variety of Bavarian dialects.Austria initially emerged as a margraviate around 976 and developed into a duchy and archduchy. In the 16th century, Austria started serving as the heart of the Habsburg Monarchy and the junior branch of the House of Habsburg – one of the most influential royal dynasties in history. As an archduchy, it was a major component and administrative centre of the Holy Roman Empire. Early in the 19th century, Austria established its own empire, which became a great power and the leading force of the German Confederation but pursued its own course independently of the other German states. Following the Austro-Prussian War and the compromise with Hungary, the Dual Monarchy was established.</t>
+          <t>Cornelis Pieter "Pete" Hoekstra (; born October 30, 1953) is a Dutch-American politician serving as the United States Ambassador to the Netherlands since January 10, 2018. A member of the Republican Party, he previously served as the U.S. Representative for Michigan's 2nd congressional district from 1993 to 2011.</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -942,17 +942,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Armenia</t>
+          <t>Jamie McCourt</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Armenia  is officially the Republic of Armenia. It is a country in the South Caucasus region of Eurasia. It is in Eastern Europe on the Armenian Highlands,</t>
+          <t>Jamie D. McCourt (born December 5, 1953) is a businesswoman and investor. She is the founder and CEO of Jamie Enterprises, and the former co-owner and executive of the Los Angeles Dodgers. She became the highest-ranking woman in Major League Baseball, appointed first as Vice Chairman of the Dodgers in 2004, then President in 2005, and finally CEO in 2009. On June 22, 2017, she was nominated as United States Ambassador to Belgium.On August 2, 2017, President Trump formally withdrew her nomination and instead nominated her as United States Ambassador to France and United States Ambassador to Monaco. This nomination was confirmed by the United States Senate on November 2, 2017.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Armenia ( (listen); Armenian: Հայաստան, romanized: Hayastan, IPA: [hɑjɑsˈtɑn]), officially the Republic of Armenia (Armenian: Հայաստանի Հանրապետություն, romanized: Hayastani Hanrapetut'yun, IPA: [hɑjɑstɑˈni hɑnɾɑpɛtutʰˈjun]), is a landlocked country in the South Caucasus region of Eurasia. Located in Western Asia, on the Armenian Highlands, it is bordered by Turkey to the west, Georgia to the north, the de facto independent Republic of Artsakh and Azerbaijan to the east, and Iran and Azerbaijan's exclave of Nakhchivan to the south.Armenia is a unitary, multi-party, democratic nation-state with an ancient cultural heritage. Urartu was established in 860 BC and by the 6th century BC it was replaced by the Satrapy of Armenia. The Kingdom of Armenia reached its height under Tigranes the Great in the 1st century BC and became the first state in the world to adopt Christianity as its official religion in the late 3rd or early 4th century AD. The official date of state adoption of Christianity is 301. The ancient Armenian kingdom was split between the Byzantine and Sasanian Empires around the early 5th century. Under the Bagratuni dynasty, the Bagratid Kingdom of Armenia was restored in the 9th century. Declining due to the wars against the Byzantines, the kingdom fell in 1045 and Armenia was soon after invaded by the Seljuk Turks. An Armenian principality and later a kingdom Cilician Armenia was located on the coast of the Mediterranean Sea between the 11th and 14th centuries.</t>
+          <t>Jamie D. McCourt (née Luskin; born December 5, 1953) is the United States Ambassador to the French Republic and Principality of Monaco. She was confirmed by the Senate and sworn in on November 2, 2017. Ambassador McCourt is also the United States Permanent Observer to the Council of Europe. McCourt is the founder and CEO of Jamie Enterprises and a former executive of the Los Angeles Dodgers. She became the highest-ranking woman in Major League Baseball, appointed first as vice chairman of the Dodgers in 2004, then President in 2005, and finally CEO in 2009.</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -962,17 +962,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Archaeology</t>
+          <t>Steve King (businessman)</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Archaeology, or archeology, is the study of the past by looking for the remains and objects left by the people who lived long ago. These remains can include old coins, tools, buildings, and inscriptions. Archaeologists, the people who study archaeology, use these remains to understand how people lived.</t>
+          <t>Steve King (born July 4, 1941) is an American businessman and Republican Party activist. He is the founder of King Capital LLC, an equity investment and real estate company. He is a former FBI agent.In 1988, he campaigned unsuccessfully for the Republican U.S. Senate nomination in Wisconsin.In July 2017, President Donald Trump nominated King to be the next United States Ambassador to the Czech Republic. This nomination was confirmed by the U.S. Senate on October 5, 2017.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Archaeology, or archeology, is the study of human activity through the recovery and analysis of material culture. The archaeological record consists of artifacts, architecture, biofacts or ecofacts and cultural landscapes. Archaeology can be considered both a social science and a branch of the humanities. In Europe it is often viewed as either a discipline in its own right or a sub-field of other disciplines, while in North America archaeology is a sub-field of anthropology.Archaeologists study human prehistory and history, from the development of the first stone tools at Lomekwi in East Africa 3.3 million years ago up until recent decades. Archaeology is distinct from palaeontology, which is the study of fossil remains. It is particularly important for learning about prehistoric societies, for whom there may be no written records to study. Prehistory includes over 99% of the human past, from the Paleolithic until the advent of literacy in societies across the world. Archaeology has various goals, which range from understanding culture history to reconstructing past lifeways to documenting and explaining changes in human societies through time.The discipline involves surveying, excavation and eventually analysis of data collected to learn more about the past. In broad scope, archaeology relies on cross-disciplinary research. It draws upon anthropology, history, art history, classics, ethnology, geography, geology, literary history, linguistics, semiology, sociology, textual criticism, physics, information sciences, chemistry, statistics, paleoecology, paleography, paleontology, paleozoology, and paleobotany.Archaeology developed out of antiquarianism in Europe during the 19th century, and has since become a discipline practiced across the world. Archaeology has been used by nation-states to create particular visions of the past. Since its early development, various specific sub-disciplines of archaeology have developed, including maritime archaeology, feminist archaeology and archaeoastronomy, and numerous different scientific techniques have been developed to aid archaeological investigation. Nonetheless, today, archaeologists face many problems, such as dealing with pseudoarchaeology, the looting of artifacts, a lack of public interest, and opposition to the excavation of human remains.</t>
+          <t>Stephen B. King (born July 4, 1941) is an American businessman and political activist serving as the United States Ambassador to the Czech Republic since 2017. A member of the Republican Party, he is the founder of King Capital LLC, an equity investment and real estate company. He previously worked at the Federal Bureau of Investigation (FBI) as an agent and campaigned unsuccessfully in 1988 for his party's nomination for the U.S. Senate in Wisconsin.</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -982,17 +982,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Application</t>
+          <t>Sharon Day</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>The word application has several uses.</t>
+          <t>Sharon Day is an American politician. She is the former co-chairwoman of the Republican National Committee.On August 3, 2017, she was confirmed as the next United States Ambassador to Costa Rica. She was nominated by President Donald Trump. She took office on September 25, 2017.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Application may refer to:</t>
+          <t>Sharon Day is the United States Ambassador to Costa Rica. She previously served as the co-chairwoman of the Republican National Committee.</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1002,17 +1002,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Animalia</t>
+          <t>Kelly Knight Craft</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Animalia is a kingdom of multicellular eukaryotic organisms. Animalia has eukaryotic organisms with many cells. They do not use light to get energy as plants do. Animals use different ways to get energy from other living things. They may eat other living things, though some are parasites or have photosynthetic protists as symbionts.</t>
+          <t>Kelly Dawn Knight Craft (née Guilfoil; born February 24, 1962) is an American diplomat. She is the 30th and current United States Ambassador to the United Nations since September 2019. Before, she was the United States ambassador to Canada, the first woman to hold the post.In 2007, she was appointed by President George W. Bush as the U.S. delegate to the United Nations, where her focus included U.S. engagement in Africa. Knight-Craft was a delegate to the 2016 Republican National Convention from Kentucky. She is a member of the University of Kentucky's board of directors. She heads Kelly G. Knight LLC, a business advisory firm based in Lexington, Kentucky.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Animals (also called Metazoa) are multicellular eukaryotic organisms that form the biological kingdom Animalia. With few exceptions, animals consume organic material, breathe oxygen, are able to move, can reproduce sexually, and grow from a hollow sphere of cells, the blastula, during embryonic development. Over 1.5 million living animal species have been described—of which around 1 million are insects—but it has been estimated there are over 7 million animal species in total. Animals range in length from 8.5 micrometres (0.00033 in) to 33.6 metres (110 ft). They have complex interactions with each other and their environments, forming intricate food webs. The kingdom Animalia includes humans but in colloquial use the term animal often refers only to non-human animals. The scientific study of animals is known as zoology.</t>
+          <t>Kelly Dawn Craft (née Guilfoil; born February 24, 1962) is an American diplomat who currently serves as the United States Ambassador to the United Nations. Craft previously served as the United States ambassador to Canada, being the first woman to hold the office. She was appointed by President George W. Bush as a U.S. alternate delegate to the United Nations in 2007, where her focus included U.S. engagement in Africa. She was a delegate to the 2016 Republican National Convention from Kentucky. She headed Kelly G. Knight LLC, a business advisory firm based in Lexington, Kentucky.She was confirmed by the U.S. Senate in a vote of 56-34, and was officially sworn in as the United Nations Ambassador on September 10, 2019. She formally presented her credentials to Secretary-General António Guterres on September 12, 2019.</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1022,17 +1022,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Animal</t>
+          <t>Doug Manchester</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Animalia is a kingdom of multicellular eukaryotic organisms. Animalia has eukaryotic organisms with many cells. They do not use light to get energy as plants do. Animals use different ways to get energy from other living things. They may eat other living things, though some are parasites or have photosynthetic protists as symbionts.</t>
+          <t>Douglas Frederick "Doug" Manchester (born June 3, 1942) is an American businessman and philanthropist. He is the former chairman of Manchester Financial Group, past chairman and publisher of The San Diego Union-Tribune. He is the nominee to become United States Ambassador to the Bahamas.Manchester has built some of the tallest hotels and office buildings in San Diego, including the San Diego Marriott Marquis &amp; Marina and the Manchester Grand Hyatt, and is credited as a driving force behind the development of the San Diego Convention Center. Manchester also built the triple 5-star Grand Del Mar Resort &amp; Spa, which sold to Fairmont Hotels &amp; Resorts in 2015, and he maintains a minority ownership.Manchester built the Torrey Executive Centre, Manchester Financial Building, Whitetail Lodge and Golf Club, and is currently building the Fairmont Austin hotel in Austin, Texas.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Animals (also called Metazoa) are multicellular eukaryotic organisms that form the biological kingdom Animalia. With few exceptions, animals consume organic material, breathe oxygen, are able to move, can reproduce sexually, and grow from a hollow sphere of cells, the blastula, during embryonic development. Over 1.5 million living animal species have been described—of which around 1 million are insects—but it has been estimated there are over 7 million animal species in total. Animals range in length from 8.5 micrometres (0.00033 in) to 33.6 metres (110 ft). They have complex interactions with each other and their environments, forming intricate food webs. The kingdom Animalia includes humans but in colloquial use the term animal often refers only to non-human animals. The scientific study of animals is known as zoology.</t>
+          <t>Douglas Frederick Manchester (born June 3, 1942) is an American businessman and philanthropist. He is the former chairman of Manchester Financial Group, past chairman and publisher of The San Diego Union-Tribune, and an unsuccessful nominee to become United States Ambassador to the Bahamas. Manchester, who prefers to be called "Papa Doug", has built some of the tallest hotels and office buildings in San Diego, including the San Diego Marriott Marquis &amp; Marina and the Manchester Grand Hyatt, and is credited as a driving force behind the development of the San Diego Convention Center. Manchester also built the triple 5-star Grand Del Mar Resort &amp; Spa, which was sold to Fairmont Hotels &amp; Resorts in 2015, and he maintains a minority ownership. Manchester also built the Torrey Executive Centre, Manchester Financial Building, Whitetail Lodge and Golf Club, Fairmont Austin and is currently building the Manchester Pacific Gateway.Manchester has long been involved in conservative politics and with the Republican Party. In late 2019, the Republican National Committee cut all ties with Manchester after CBS News obtained emails between Manchester, Ronna McDaniel, and GOP senate staffers in which Manchester appeared to be engaged in a pay-to-play scheme.</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1042,17 +1042,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Acceleration</t>
+          <t>John R. Bass</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Acceleration is a measure of how fast velocity changes. Acceleration is the change of velocity divided by the change of time. Acceleration is a vector, and therefore includes both a size and a direction. Acceleration is also a change in speed and direction, there is:</t>
+          <t>John R. Bass (born 1964) is an American diplomat. He is the current United States Ambassador to Afghanistan since December 2017. He served as the United States Ambassador to Turkey from 2014 to 2016. He was United States Ambassador to Georgia from 2009 to 2012.President Donald Trump named him as his choice to become the United States Ambassador to Afghanistan on July 20, 2017. On September 28, 2017, his nomination was confirmed by the Senate.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>In mechanics, acceleration is the rate of change of the velocity of an object with respect to time.</t>
+          <t>John Rodney Bass II (born 1964) is an American diplomat, who served as the United States Ambassador to Afghanistan from 2017 to 2020. He was the U.S. ambassador to Turkey 2014–2017 and the U.S. ambassador to Georgia 2009–2012.</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1062,17 +1062,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Black pudding</t>
+          <t>Jeffrey Dean Morgan</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Black pudding is an English name for zwarte pudding.  It is food made by cooking down the blood of any mammal (usually pigs or cattle) with meat, fat or filler until it is thick enough to congeal (become firm or solid) when cooled.</t>
+          <t xml:space="preserve">Jeffrey Dean Morgan (born April 22, 1966) is an American actor. He is known for playing John Winchester on Supernatural, Denny Duquette on the medical drama Grey's Anatomy, The Comedian in the 2009 superhero movie Watchmen, Jason Crouse on The Good Wife, and Negan on The Walking Dead. </t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Black pudding is a distinct regional type of blood sausage originating in the United Kingdom and Ireland. It is made from pork blood, with pork fat or beef suet, and a cereal, usually oatmeal, oat groats or barley groats. The high proportion of cereal, along with the use of certain herbs such as pennyroyal, serves to distinguish black pudding from blood sausages eaten in other parts of the world.</t>
+          <t>Jeffrey Dean Morgan is an American actor of film and television. He is known for his roles as John Winchester in the fantasy horror series Supernatural (2005–2007; 2019), Denny Duquette in the medical drama series Grey's Anatomy (2006–2009), the Comedian in the superhero film Watchmen (2009), Jason Crouse in the political drama series The Good Wife (2015–2016), Negan in the horror drama series The Walking Dead (2016–present), and Harvey Russell in Rampage (2018).</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1082,17 +1082,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Boot device</t>
+          <t>Lauren Cohan</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>A boot device is used to start a computer.  It is named after a boot which fits on the foot.  The word bootstrap is also closely related, and means, to use something simpler to get something more complex to make itself work better. It comes from the English phrase "pull yourself up by your own bootstraps."</t>
+          <t>Lauren Cohan (born January 7, 1982) is a British American actress and model.Cohan best known for her role as Maggie Rhee on The Walking Dead (2011–present). She is also known for her recurring roles on the television series Supernatural (2007–2008), Chuck (2011) and The Vampire Diaries (2010–2012), and in the comedy movie Van Wilder: The Rise of Taj (2006), the psychological thriller The Boy, and for her role in the DC Extended Universe as character Martha Wayne in Batman v Superman: Dawn of Justice (2016).</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">In computing, booting is the process of starting a computer. It can be initiated by hardware such as a button press, or by a software command. After it is switched on, a computer's central processing unit (CPU) has no software in its main memory, so some process must load software into memory before it can be executed.  This may be done by hardware or firmware in the CPU, or by a separate processor in the computer system. </t>
+          <t>Lauren Cohan (born January 7, 1982) is an American–English actress best known for her role as Maggie Greene in the horror television series The Walking Dead (2011–2018, 2020). Her other notable TV roles include Bela Talbot in the fantasy-horror series Supernatural (2007–2008), Rose in the supernatural series The Vampire Diaries (2010–2012), Vivian McArthur Volkoff in the action comedy series Chuck (2007), and  Francesca 'Frankie' Trowbridge in the spy drama Whiskey Cavalier (2019). Her film appearances include the comedy Van Wilder: The Rise of Taj (2006), the psychological thriller horror The Boy (2016), the biographical drama All Eyez on Me (2017), and the action thriller Mile 22 (2018).</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1102,17 +1102,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Boot</t>
+          <t>Ben Ferencz</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>A boot is a type of footwear that protects the foot and ankle. Boots are higher and larger than shoes and sandals. Some boots are high enough to protect the calves (lower part of the leg) as well.  Some boots are held on with bootstraps or bootlaces.  Some also have spats or gaiters to keep water out.  Most have a very strong boot sole, the bottom part of a boot.</t>
+          <t>Benjamin Berell Ferencz (born March 11, 1920) is a Romanian-born American lawyer of Hungarian-Jewish descent. He was an investigator of Nazi war crimes after World War II and the Chief Prosecutor for the United States Army at the Einsatzgruppen Trial, one of the twelve military trials held by the U.S. authorities at Nuremberg, Germany.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>A boot, plural boots, is a type of specific footwear. Most boots mainly cover the foot and the ankle, while some also cover some part of the lower calf. Some boots extend up the leg, sometimes as far as the knee or even the hip. Most boots have a heel that is clearly distinguishable from the rest of the sole, even if the two are made of one piece. Traditionally made of leather or rubber, modern boots are made from a variety of materials. Boots are worn both for their functionality – protecting the foot and leg from water, extreme cold, mud or hazards (e.g., work boots may protect wearers from chemicals or use a steel toe) or providing additional ankle support for strenuous activities with added traction requirements (e.g., hiking), or may have hobnails on their undersides to protect against wear and to get better grip; and for reasons of style and fashion.</t>
+          <t>Benjamin Berell Ferencz (born March 11, 1920) is an American lawyer. He was an investigator of Nazi war crimes after World War II and the chief prosecutor for the United States Army at the Einsatzgruppen Trial, one of the 12 military trials held by the U.S. authorities at Nuremberg, Germany. Later, he became an advocate of the establishment of an international rule of law and of an International Criminal Court. From 1985 to 1996, he was adjunct professor of international law at Pace University.</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1122,17 +1122,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Bankruptcy</t>
+          <t>Benjamin Ferencz</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Bankruptcy is a legal process which happens when a person or an organisation does not have enough money to pay all of its debts.  Legally they are insolvent.</t>
+          <t>Benjamin Berell Ferencz (born March 11, 1920) is a Romanian-born American lawyer of Hungarian-Jewish descent. He was an investigator of Nazi war crimes after World War II and the Chief Prosecutor for the United States Army at the Einsatzgruppen Trial, one of the twelve military trials held by the U.S. authorities at Nuremberg, Germany.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Bankruptcy is a legal process through which people or other entities who cannot repay debts to creditors may seek relief from some or all of their debts. In most jurisdictions, bankruptcy is imposed by a court order, often initiated by the debtor.</t>
+          <t>Benjamin Berell Ferencz (born March 11, 1920) is an American lawyer. He was an investigator of Nazi war crimes after World War II and the chief prosecutor for the United States Army at the Einsatzgruppen Trial, one of the 12 military trials held by the U.S. authorities at Nuremberg, Germany. Later, he became an advocate of the establishment of an international rule of law and of an International Criminal Court. From 1985 to 1996, he was adjunct professor of international law at Pace University.</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1142,17 +1142,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Breakfast sausage</t>
+          <t>Stanislav Lyubshin</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Breakfast sausage is a type of fresh pork sausage made from seasoned ground meat mixed with bread crumbs. Breakfast sausage has a blander flavor than many other types of sausage, such as British or Italian-style sausages.</t>
+          <t>Stanislav Andreyevich Lyubshin (Russian: Станисла́в Андре́евич Любшин; born 6 April 1933) is a Russian actor, screenwriter and movie director. He was awarded the People's Artist of the RSFSR in 1981. His debut movie was Shchit i mech (1968). From 1964 to 1967, he was member of the Taganka Theatre company in Moscow. Since 1981 Lyubshin has been permanent member with the Moscow Art Theatre (MKhAT named after A. Chekhov).</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Breakfast sausage (or country sausage) is a type of fresh pork sausage usually served at breakfast in the United States. It is a common breakfast item in traditional American "farmer" or "country" breakfasts, as it originated as a way for farmers to make use of as much of their livestock (usually pigs) as possible. Scraps and trimmings were ground, seasoned and later consumed by the farmer as an inexpensive, high-protein morning meal.It is perhaps most popular for home consumption in rural areas, particularly in the southern states, where it is in the form of fresh or smoked patties or links (the latter might have a natural or synthetic casing, or no form of any casing). Most diners, fast-food restaurants, and family restaurants across the country will also carry one or more versions of it during breakfast hours, whether on a sandwich, in a breakfast platter, or both; some fine-dining establishments will also have a sausage option on their breakfast or brunch menu.The cased link variety is most similar to English-style sausages and has been produced in the United States since colonial days. It is essentially a highly seasoned ground meat, so it does not keep and should be stored and handled appropriately. Newer variations made from pork and beef mixtures as well as poultry can also be found. There are also vegetarian varieties that use textured vegetable protein in place of meat.  In the United States, the predominant flavorings used for seasoning are black pepper or white pepper and sage, although there are varieties also seasoned with cayenne pepper, or even maple syrup. Some breakfast sausage is flavored with cured bacon.Breakfast sausage is normally fried in a pan, grilled, or microwaved. Some people like to put maple syrup onto their breakfast sausages.  Cooked breakfast sausage is also mixed into egg casseroles before baking. Crumbled and added to white gravy, it is a central component of sausage gravy.</t>
+          <t>Stanislav Andreyevich Lyubshin (Russian: Станислав Андреевич Любшин; born 6 April 1933) is a Russian actor, film director, and People's Artist of the RSFSR (1981).</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1162,17 +1162,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Browser</t>
+          <t>Eberhard Jäckel</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>A browser is an animal, usually a herbivorous mammal, which eats leaves and shrubs rather than grass. It is contrasted with grazers, which eat grass.</t>
+          <t>Eberhard Jäckel (June 29, 1929 – August 15, 2017) was a Social Democratic German historian. He was known for his studies of Adolf Hitler's role in German history. Jäckel sees Hitler as being the historical equivalent to the Chernobyl disaster.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Browse, browser or browsing may refer to:</t>
+          <t>Eberhard Jäckel (29 June 1929 – 15 August 2017) was a Social Democratic German historian, noted for his studies of Adolf Hitler's role in German history. Jäckel sees Hitler as being the historical equivalent to the Chernobyl disaster.</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1182,17 +1182,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Beekeeping</t>
+          <t>Gueberschwihr</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Beekeeping or apiculture is the farming of honeybees.</t>
+          <t>Gueberschwihr is a commune. It is found in the Haut-Rhin department of eastern France.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Beekeeping (or apiculture) is the maintenance of bee colonies, commonly in man-made hives, by humans. Most such bees are honey bees in the genus Apis, but other honey-producing bees such as Melipona stingless bees are also kept. A beekeeper (or apiarist) keeps bees in order to collect their honey and other products that the hive produce (including beeswax, propolis, flower pollen, bee pollen, and royal jelly), to pollinate crops, or to produce bees for sale to other beekeepers. A location where bees are kept is called an apiary or "bee yard".</t>
+          <t>Gueberschwihr (Alemannic German: Gawerschwihr; German: Geberschweier) is a commune in the Haut-Rhin department in Grand Est in north-eastern France.</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1202,17 +1202,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>British English</t>
+          <t>Citroën Jumpy</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>British English is the kind of English language which is used in the United Kingdom and in most countries which previously were in the British Empire.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>British English is the standard dialect of the English language as spoken and written in the United Kingdom. Variations exist in formal, written English in the United Kingdom. For example, the adjective wee is almost exclusively used in parts of Scotland, North East England, Ireland, and occasionally Yorkshire, whereas little is predominant elsewhere. Nevertheless, there is a meaningful degree of uniformity in written English within the United Kingdom, and this could be described by the term British English.  The forms of spoken English, however, vary considerably more than in most other areas of the world where English is spoken, so a uniform concept of British English is more difficult to apply to the spoken language. According to Tom McArthur in the Oxford Guide to World English, British English shares "all the ambiguities and tensions in the word 'British' and as a result can be used and interpreted in two ways, more broadly or more narrowly, within a range of blurring and ambiguity".Colloquial portmanteau words for British English include: Bringlish (recorded from 1967), Britglish (1973), Britlish (1976), Brenglish (1993) and Brilish (2011).</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1222,17 +1222,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Being</t>
+          <t>Citroen Jumpy</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Being is also a present tense part of to beThe word being means a living person or animal. ‘Human being’ means the same as ’person’. Men, women, and children are human beings.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>In philosophy, being means the material or immaterial existence of a thing. Anything that exists is being. Ontology is the branch of philosophy that studies being. Being is a concept encompassing objective and subjective features of reality and existence. Anything that partakes in being is also called a "being", though often this usage is limited to entities that have subjectivity (as in the expression "human being"). The notion of "being" has, inevitably, been elusive and controversial in the history of philosophy, beginning in Western philosophy with attempts among the pre-Socratics to deploy it intelligibly. The first effort to recognize and define the concept came from Parmenides, who famously said of it that "what is-is". Common words such as "is", "are", and "am" refer directly or indirectly to being.</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1242,17 +1242,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Bootstrap</t>
+          <t>Citroen Space Tourer</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>A boot is a type of footwear that protects the foot and ankle. Boots are higher and larger than shoes and sandals. Some boots are high enough to protect the calves (lower part of the leg) as well.  Some boots are held on with bootstraps or bootlaces.  Some also have spats or gaiters to keep water out.  Most have a very strong boot sole, the bottom part of a boot.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Bootstrapping is a self-starting process that is supposed to proceed without external input.</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1262,17 +1262,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Bootlace</t>
+          <t>Citroen Spacetourer</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>A boot is a type of footwear that protects the foot and ankle. Boots are higher and larger than shoes and sandals. Some boots are high enough to protect the calves (lower part of the leg) as well.  Some boots are held on with bootstraps or bootlaces.  Some also have spats or gaiters to keep water out.  Most have a very strong boot sole, the bottom part of a boot.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Shoelaces, also called shoestrings (US English) or bootlaces (UK English), are a system commonly used to secure shoes, boots, and other footwear. They typically consist of a pair of strings or cords, one for each shoe, finished off at both ends with stiff sections, known as aglets. Each shoelace typically passes through a series of holes, eyelets, loops or hooks on either side of the shoe. Loosening the lacing allows the shoe to open wide enough for the foot to be inserted or removed. Tightening the lacing and tying off the ends secures the foot firmly within the shoe.</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1282,17 +1282,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Beijing</t>
+          <t>Citroen Dispatch</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Beijing is the capital of the People's Republic of China. The city used to be known as Peking.  It is in the northern and eastern parts of the country. It is the world's most populous capital city.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Beijing ( BAY-JING,  BAY-ZHING; Mandarin pronunciation: [pèi.tɕíŋ] (listen)), alternatively romanized as Peking ( PEY-KING), is the capital of the People's Republic of China. It is the world's most populous capital city, with over 21 million residents within an administrative area of 16,410.5 km2. The city, located in North China, is governed as a municipality under the direct administration of the central government with 16 urban, suburban, and rural districts. Beijing is mostly surrounded by Hebei Province with the exception of neighboring Tianjin to the southeast; together, the three divisions form the Jingjinji megalopolis and the national capital region of China.</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1302,17 +1302,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Bottle</t>
+          <t>Citroën Dispatch</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>A bottle is a container used to carry liquids. Bottles can have many different sizes. Bottles are usually made of glass or plastic. Usually, Beer bottles are made of glass, and soft drinks are made of plastic.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>A bottle is a narrow-necked container made of an impermeable material (clay, glass, plastic, aluminium etc.) in various shapes and sizes  to store and transport liquids (water, milk, beer, wine, ink, cooking oil, medicine, soft drinks, shampoo, and chemicals, etc.) and whose mouth at the bottling line can be sealed with an internal stopper, an external bottle cap, a closure, or a conductive "inner seal" using induction sealing.</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1322,17 +1322,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Berry</t>
+          <t>Citroën Space Tourer</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>The word berry is used for many different kinds of small fruits that have many seeds and can be used as food. Some examples are raspberry, strawberry, lingonberry and blueberry.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve">A berry is a small, pulpy, and often edible fruit. Typically, berries are juicy, rounded, brightly colored, sweet, sour or tart, and do not have a stone or pit, although many pips or seeds may be present. Common examples are strawberries, raspberries, blueberries, blackberries, red currants, white currants and blackcurrants. In Britain, soft fruit is a horticultural term for such fruits.In common usage, the term "berry" differs from the scientific or botanical definition of a fruit produced from the ovary of a single flower in which the outer layer of the ovary wall develops into an edible fleshy portion (pericarp). The botanical definition includes many fruits that are not commonly known or referred to as berries, such as grapes, tomatoes, cucumbers, eggplants, bananas, and chili peppers. Fruits commonly considered berries but excluded by the botanical definition include strawberries, raspberries, and blackberries, which are aggregate fruits and mulberries, which are multiple fruits. Watermelons and pumpkins are giant berries that fall into the category "pepos". A plant bearing berries is said to be bacciferous or baccate. </t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1342,17 +1342,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Boil</t>
+          <t>Citroën Spacetourer</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Boil might mean:</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>A boil, also called a furuncle, is a deep folliculitis, infection of the hair follicle. It is most commonly caused by infection by the bacterium Staphylococcus aureus, resulting in a painful swollen area on the skin caused by an accumulation of pus and dead tissue. Boils which are expanded are basically pus-filled nodules. Individual boils clustered together are called carbuncles.</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1362,17 +1362,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>Citroёn Space Tourer</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>A beard is the hair growing on the lower part of a man's face.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>A beard is the hair that grows on the chin, upper lip, cheeks and neck of humans and some non-human animals. In humans, usually only pubescent or adult males are able to grow beards. Some women with hirsutism, a hormonal condition of excessive hairiness, may develop a beard.</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1382,17 +1382,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Peugeot Expert</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>In light, black is lack of all color.  In painting, however, the black pigment is the combination of all colors. In heraldry, black is called "sable". It is the opposite of white.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Black is the darkest color, the result of the absence or complete absorption of visible light. It is an achromatic color, a color without hue, like white and gray. It is often used symbolically or figuratively to represent darkness, while white represents light. Black and white have often been used to describe opposites such as good and evil, the Dark Ages versus Age of Enlightenment, and night versus day. Since the Middle Ages, black has been the symbolic color of solemnity and authority, and for this reason is still commonly worn by judges and magistrates.Black was one of the first colors used by artists in neolithic cave paintings. In the 14th century, it was worn by royalty, clergy, judges and government officials in much of Europe. It became the color worn by English romantic poets, businessmen and statesmen in the 19th century, and a high fashion color in the 20th century. In the Roman Empire, it became the color of mourning, and over the centuries it was frequently associated with death, evil, witches and magic. According to surveys in Europe and North America, it is the color most commonly associated with mourning, the end, secrets, magic, force, violence, evil, and elegance.Black ink is the most common color used for printing books, newspapers and documents, as it provides the highest contrast with white paper and thus the easiest color to read. Similarly, black text on a white screen is the most common format used on computer screens.</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1402,17 +1402,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Bubonic plague</t>
+          <t>Peugeot Expert Tepee</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Bubonic plague is the best-known form of the disease plague, which is caused by the bacterium Yersinia pestis. The name bubonic plague is specific for this form of the disease, which enters through the skin, and travels through the lymphatic system.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Bubonic plague is one of three types of plague caused by bacterium Yersinia pestis. One to seven days after exposure to the bacteria, flu-like symptoms develop. These symptoms include fever, headaches, and vomiting. Swollen and painful lymph nodes occur in the area closest to where the bacteria entered the skin. Occasionally, the swollen lymph nodes may break open.The three types of plague are the result of the route of infection: bubonic plague, septicemic plague, and pneumonic plague. Bubonic plague is mainly spread by infected fleas from small animals. It may also result from exposure to the body fluids from a dead plague-infected animal. In the bubonic form of plague, the bacteria enter through the skin through a flea bite and travel via the lymphatic vessels to a lymph node, causing it to swell. Diagnosis is made by finding the bacteria in the blood, sputum, or fluid from lymph nodes.Prevention is through public health measures such as not handling dead animals in areas where plague is common. Vaccines have not been found to be very useful for plague prevention. Several antibiotics are effective for treatment, including streptomycin, gentamicin, and doxycycline. Without treatment, plague results in the death of 30% to 90% of those infected. Death, if it occurs, is typically within ten days. With treatment the risk of death is around 10%. Globally between 2010 and 2015 there were 3248 documented cases, which resulted in 584 deaths. The countries with the greatest number of cases are the Democratic Republic of the Congo, Madagascar, and Peru.The plague was the cause of the Black Death that swept through Asia, Europe, and Africa in the 14th century and killed an estimated 50 million people. This was about 25% to 60% of the European population. Because the plague killed so many of the working population, wages rose due to the demand for labor. Some historians see this as a turning point in European economic development. The disease was also responsible for the Justinian plague originating in the Eastern Roman Empire in the 6th century CE, as well as the third epidemic affecting China, Mongolia, and India originating in the Yunnan Province in 1855. The term bubonic is derived from the Greek word βουβών, meaning "groin". The term "buboes" is also used to refer to the swollen lymph nodes.</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1422,17 +1422,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Biology</t>
+          <t>Peugeot Traveller</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Biology is the science that studies life, and living things, and the evolution of life. Living things include animals, plants, fungi (such as mushrooms), and microorganisms such as bacteria and archaea.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Biology is the natural science that studies life and living organisms, including their physical structure, chemical processes, molecular interactions, physiological mechanisms, development and evolution. Despite the complexity of the science, there are certain unifying concepts that consolidate it into a single, coherent field. Biology recognizes the cell as the basic unit of life, genes as the basic unit of heredity, and evolution as the engine that propels the creation and extinction of species. Living organisms are open systems that survive by transforming energy and decreasing their local entropy to maintain a stable and vital condition defined as homeostasis.Sub-disciplines of biology are defined by the research methods employed and the kind of system studied: theoretical biology uses mathematical methods to formulate quantitative models while experimental biology performs empirical experiments to test the validity of proposed theories and understand the mechanisms underlying life and how it appeared and evolved from non-living matter about 4 billion years ago through a gradual increase in the complexity of the system. See branches of biology.</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1442,17 +1442,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Daniel Catan</t>
+          <t>Toyota ProAce</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Daniel Catán Porteny (3 April 1949 in Mexico City - 9 April 2011 in Austin, Texas) was a Mexican opera composer of Jewish descent. He is best known for turning the Italian movie, Il Postino, into an opera. He was working at the University of Texas at Austin on a new opera based on the Frank Capra movie, Meet John Doe.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Daniel Catán (April 3, 1949 – April 9, 2011) was a Mexican composer, writer and professor known particularly for his operas and his contribution of the Spanish language to the international repertory.With a compositional style described as lush, romantic and lyrical, Catán’s second opera, Rappaccini’s Daughter, became the first Mexican opera in the United States to be produced by a professional opera company.  Upon receiving international recognition, Catán’s next opera, Florencia en el Amazonas, became the first opera in Spanish to be commissioned by an opera company in the United States.  Shortly after, Catán received a Plácido Domingo Award and a Guggenheim Fellowship Award for his contributions to music.  In 2004, Catán’s opera Salsipuedes: a Tale of Love, War and Anchovies was premiered by the Houston Grand Opera.  In September 2010, his opera Il Postino was premiered by the Los Angeles Opera with Plácido Domingo singing as Pablo Neruda, a role written specifically for him.  Catán died while working on his next opera, Meet John Doe.Catán’s works also include vocal, chamber, orchestral and choral music as well as music for ballet, film and TV.</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1462,17 +1462,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Blue eyed soul</t>
+          <t>Toyota Proace</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Blue Eyed Soul is a term used to describe Soul and R&amp;B music sung by white people. The term was first used in the 1960s about white artists performing music which was similar to the music being performed by Motown artists. It is sometimes called white soul.</t>
+          <t>The Citroën Jumpy (Citroën Dispatch in some countries) is a series of vans and passenger vans produced by Citroën in three generations since 1994. It is builded in cooperation with Fiat and Peugeot.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Blue-eyed soul (also known as white soul) is rhythm and blues and soul music performed by white artists.  The term was coined in the mid-1960s, to describe white artists who performed soul and R&amp;B that was similar to the music of the Motown and Stax record labels.  Though many rhythm and blues radio stations in the United States in that period would only play music by black musicians, some began to play music by white acts considered to have "soul feeling" and their music was then described as "blue-eyed soul".</t>
+          <t>The Citroën Jumpy (badged Citroën Dispatch in some countries) is a light commercial van produced at Sevel Nord since 1994. The Jumpy was also sold as the Peugeot Expert and Fiat Scudo beginning in 1995.</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1482,17 +1482,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Monte dei Paschi di Siena</t>
+          <t>Sonny Landham</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Banca Monte dei paschi di Siena (sometimes referred to as BMPS or MPS) claims to be the oldest surviving retail bank in the world. It has its headquarters in Siena, Italy.</t>
+          <t>William M. "Sonny" Landham (February 11, 1941 – August 17, 2017) was an American actor, stunt man and politician. He played tracker Billy Sole in the action movie Predator.Landham was born in Canton, Georgia. He studied at the University of Georgia.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Banca Monte dei Paschi di Siena S.p.A. (Italian pronunciation: [ˈbaŋka ˈmonte dei ˈpaski di ˈsjɛːna]), known as BMPS or just MPS, is an Italian bank. Tracing its history to a mount of piety founded in 1472 (548 years ago) and founded in its present form in 1624 (396 years ago), it is the world's oldest or second oldest bank, depending on the definition, and the fourth largest Italian commercial and retail bank.In 1995 the bank, then known as Monte dei Paschi di Siena, was transformed from a statutory corporation to a limited company called Banca Monte dei Paschi di Siena (Banca MPS). The Fondazione Monte dei Paschi di Siena was created to continue the charitable functions of the bank and to be, until the bailout in 2013, its largest single shareholder. Today Banca MPS has approximately 2,000 branches, 26,000 employees and 5.1 million customers in Italy, as well as branches and businesses abroad. A subsidiary, MPS Capital Services, handles corporate and investment banking.According to a research by Mediobanca and a press release by Banco BPM, Banco BPM overtook BMPS as the third largest commercial banking group in Italy in terms of total assets on 31 December 2016, after Banco BPM's formal formation on 1 January 2017. In 2016–17, BMPS was struggling to avoid a collapse, and was bailed out again by the Italian government in July 2017.</t>
+          <t>William M. "Sonny" Landham (February 11, 1941 – August 17, 2017) was an American film actor and stunt man. He portrayed Billy Bear in 48 Hrs. and tracker Billy Sole in Predator.</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1502,17 +1502,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Guebwiller</t>
+          <t>Krestovsky Stadium</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Guebwiller is a commune in the Haut-Rhin department in Grand Est of eastern France.</t>
+          <t>The Saint Petersburg Stadium (Russian: Стадион Санкт-Петербург; also called the Krestovsky Stadium or Zenit Arena) is an association football stadium in Saint Petersburg, Russia. During the  2018 FIFA World Cup, the stadium had a capacity of 64,468 people. The stadium cost $1.1 billion to $1.4 billion.The stadium is now the home of FC Zenit St. Petersburg. It was used for the 2017 FIFA Confederations Cup, 2018 FIFA World Cup, and will be used for the UEFA Euro 2020.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Guebwiller (French: Guebwiller, pronounced [ɡebvilɛʁ]; Alsatian: Gàwiller [ˈkaːviləʁ]; German: Gebweiler) is a commune in the Haut-Rhin department in Grand Est currently in north-eastern France.</t>
+          <t>Krestovsky Stadium, known as Gazprom Arena for sponsorship reasons, (Russian: «Газпром Арена») is a retractable roof stadium with a retractable pitch in the western portion of Krestovsky Island in Saint Petersburg, Russia, which serves as home for FC Zenit Saint Petersburg. The stadium was opened in 2017 for the FIFA Confederations Cup. It was called Saint Petersburg Stadium during the 2017 FIFA Confederations Cup and 2018 FIFA World Cup.</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1522,17 +1522,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Natural scientists</t>
+          <t>Black-body radiation</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>There are some sciences that are used to study nature. According to these sciences, the things that can be observed in nature follow certain rules. These rules are often unknown, and natural sciences are about finding them. They often use what is called the scientific method to do this.</t>
+          <t>Blackbody radiation is radiation produced by heated objects, particularly from a blackbody. A blackbody is an object that absorbs all radiation (visible light, infrared light, ultraviolet light, etc.) that falls on it. This also means that it will also radiate at all frequencies that heat energy produces in it.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Natural science is a branch of science concerned with the description, prediction, and understanding of natural phenomena, based on empirical evidence from observation and experimentation. Mechanisms such as peer review and repeatability of findings are used to try to ensure the validity of scientific advances.</t>
+          <t>Black-body radiation is the thermal electromagnetic radiation within or surrounding a body in thermodynamic equilibrium with its environment, emitted by a black body (an idealized opaque, non-reflective body).  It has a specific spectrum of wavelengths, inversely related to intensity that depend only on the body's temperature, which is assumed for the sake of calculations and theory to be uniform and constant.The thermal radiation spontaneously emitted by many ordinary objects can be approximated as black-body radiation.  A perfectly insulated enclosure that is in thermal equilibrium internally contains black-body radiation and will emit it through a hole made in its wall, provided the hole is small enough to have a negligible effect upon the equilibrium.</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1542,17 +1542,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Morges</t>
+          <t>Abdirahman Jama Barre</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Morges is a city in the Swiss canton of Vaud. It is the capital of the district Morges.</t>
+          <t xml:space="preserve">Abdirahman Jama Barre (Somali: Cabdiraxmaan Jaamac Barre, Arabic: عبد الرحمن جامع بري‎‎) (1937 – 15 August 2017) was a Somali politician. He twice served as the Minister of Foreign Affairs of the Somali Democratic Republic, and later as the Minister of Finance. He was also the 1st Deputy Prime Minister of Somalia. He served all three positions at the same time from 1987 through 1991. </t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Morges (Latin: Morgiis, plural, probably ablative, else dative) is a municipality in the Swiss canton of Vaud and the seat of the district of Morges. It is located on Lake Geneva.</t>
+          <t>Abdirahman Jama Barre (Somali: Cabdiraxmaan Jaamac Barre, Arabic: عبد الرحمن جامع بري‎) (1937 – 15 August 2017) was a Somali politician. He twice served as the Minister of Foreign Affairs of the Somali Democratic Republic, and later as the Minister of Finance. He was also the 1st Deputy Prime Minister of Somalia.</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1562,17 +1562,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>MTS Centre</t>
+          <t>Laurie Brokenshire</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Bell MTS Place, originally known as True North Centre and later as MTS Centre, is a sports arena in Winnipeg, Manitoba, Canada. The arena opened on November 16, 2004, and is the current home to the Winnipeg Jets of the National Hockey League (NHL). The arena was originally known as True North Centre during planning but naming rights were bought by Manitoba Telecom Services (MTS). After Bell Canada purchased MTS in spring 2017, the arena was renamed effective that May 30.The arena has been home to the Manitoba Moose of the American Hockey League (AHL), the Jets' top minor-league team, two different times. The team first played there from 2004 to 2011 before moving to St. John's, Newfoundland and Labrador, and then returned to Winnipeg in 2015.</t>
+          <t>Commodore Laurence Phillip Brokenshire CBE, RN (20 October 1952 – 4 August 2017) was a British navy officer and magician. He was born in Plymouth, Devon. He studied at the University of Exeter. His career developed as a submariner and later as a senior Royal Navy officer. He retired as officer in 2003. Laurie was accepted into the Inner Magic Circle, and became an occasional professional / semi-professional magic performer.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Bell MTS Place is an indoor arena in downtown Winnipeg, Manitoba. The arena is the home of the National Hockey League's Winnipeg Jets and their American Hockey League affiliate, the Manitoba Moose.The arena stands on the former Eaton's site and is owned and operated by True North Sports &amp; Entertainment. The 440,000 square feet (41,000 m2) building was constructed at a cost of $133.5 million CAD. It opened on November 16, 2004, replacing the since-demolished Winnipeg Arena. It has a capacity of 15,321 for hockey and 16,345 for concerts.</t>
+          <t>Commodore Laurence Phillip Brokenshire CBE (1952–2017), known as Laurie Brokenshire, was a Royal Naval officer, magician and world-class puzzle solver.</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1582,17 +1582,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Varna</t>
+          <t>Pertti Alaja</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Varna is a social concept from the Brahmin leaders of Hinduism in India</t>
+          <t>Pertti Johannes Alaja (18 February 1952 – 18 August 2017) was a Finnish footballer. He was born in Helsinki, Finland. He played as a goalkeeper. He played for HJK, Haka, Oulun Työväen Palloilijat, Ikast, Edmonton Drillers, Malmö FF and for the Finland national football team.Alaja was elected as the 15th president of the Football Association of Finland on 14 October 2012, replacing Sauli Niinistö.Alaja died in Espoo, Finland, on 18 August 2017 of cancer at the age of 65.</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Varna (Bulgarian: Варна, pronounced [ˈvarnɐ]) is the third-largest city in Bulgaria and the largest city and seaside resort on the Bulgarian Black Sea Coast. Situated strategically in the Gulf of Varna, the city has been a major economic, social and cultural centre for almost three millennia. Varna, historically known as Odessos (Ancient Greek: Ὀδησσός), grew from a Thracian seaside settlement to a major seaport on the Black Sea.</t>
+          <t>Pertti Johannes Alaja (18 February 1952 – 18 August 2017) was a Finnish footballer who played as a goalkeeper.Alaja was elected as the 15th president of the Football Association of Finland on 14 October 2012, replacing Sauli Niinistö.</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1602,17 +1602,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Girard, Ohio</t>
+          <t>2017 Turku stabbings</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Girard is a city in Trumbull County, Ohio, United States. The population was 9,958 at the 2010 census. It is part of Mahoning Valley.</t>
+          <t>On 18 August 2017, around 16:00 local time (UTC+3), several people were stabbed in central Turku, Finland. Alarm was first raised at 16:02 and by 16:05 the suspect had been captured. At least two people died in the attack.</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Girard is a city in Trumbull County, Ohio, United States. The population was 9,958 at the 2010 census. It is part of the Youngstown-Warren-Boardman, OH-PA Metropolitan Statistical Area.</t>
+          <t>The 2017 Turku attack took place on 18 August 2017 at around 16:02–16:05 local time (UTC+3) when 10 people were stabbed in central Turku, Southwest Finland. Two women were killed in the attack and eight people sustained injuries. It remains the only terrorist attack ever in Finland.Police were informed at 16:02. Three minutes later the attacker, Abderrahman Bouanane, a Moroccan rejected asylum seeker, had been detained. At the time of his arrest, Bouanane was using the name Abderrahman Mechkah, which was later discovered to be a false identity. In June 2018, Bouanane was found guilty of two counts of murder with terrorist intent and eight counts of attempted murder with terrorist intent. It was the first time anybody had been sentenced for a terrorist crime in Finland.</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1622,17 +1622,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>WWE World Championship</t>
+          <t>2017 Turku stabbing</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>The WWE Championship is a professional wrestling world championship in WWE. It is the first world title of WWE. The title is said to be the biggest prize in professional wrestling and millions of people around the world watch matches for it.</t>
+          <t>On 18 August 2017, around 16:00 local time (UTC+3), several people were stabbed in central Turku, Finland. Alarm was first raised at 16:02 and by 16:05 the suspect had been captured. At least two people died in the attack.</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>The WWE Championship is a world heavyweight championship created and promoted by the American professional wrestling promotion WWE, currently defended on their Raw brand. It is one of three world titles in WWE, alongside the WWE Universal Championship on SmackDown and the NXT Championship on NXT. The current champion is Drew McIntyre, who is in his first reign.</t>
+          <t>The 2017 Turku attack took place on 18 August 2017 at around 16:02–16:05 local time (UTC+3) when 10 people were stabbed in central Turku, Southwest Finland. Two women were killed in the attack and eight people sustained injuries. It remains the only terrorist attack ever in Finland.Police were informed at 16:02. Three minutes later the attacker, Abderrahman Bouanane, a Moroccan rejected asylum seeker, had been detained. At the time of his arrest, Bouanane was using the name Abderrahman Mechkah, which was later discovered to be a false identity. In June 2018, Bouanane was found guilty of two counts of murder with terrorist intent and eight counts of attempted murder with terrorist intent. It was the first time anybody had been sentenced for a terrorist crime in Finland.</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1642,17 +1642,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Smartism</t>
+          <t>Sapa'u Ruperake Petaia</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Smartism is a sect of Hinduism in which, in contrast with Shaivism and Vaishnavism, one may worship multiple gods. It is often referred as a "liberal" sect and is passed along familial ties.</t>
+          <t xml:space="preserve">Sapa'u Ruperake Petaia (born 11 April 1951) is a Samoan poet and writer. </t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Smarta tradition (स्मार्त) is a movement in Hinduism that developed during its classical period around the beginning of the Common Era. It reflects a Hindu synthesis of four philosophical strands: Mimamsa, Advaita, Yoga, and theism. The Smarta tradition rejects theistic sectarianism, and it is notable for the domestic worship of five shrines with five deities, all treated as equal – Shiva, Vishnu, Surya, Ganesha, and Shakti. The Smarta tradition contrasted with the older Shrauta tradition, which was based on elaborate rituals and rites. There has been considerable overlap in the ideas and practices of the Smarta tradition with other significant historic movements within Hinduism, namely Shaivism, Brahmanism, Vaishnavism, and Shaktism.The Smarta tradition is aligned with Advaita Vedanta, and regards Adi Shankara as its founder or reformer. Shankara championed that the ultimate reality is impersonal and Nirguna (attributeless) and that any symbolic god serves the same equivalent purpose. Inspired by this belief, the Smarta tradition followers, along with the five Hindu gods include a sixth impersonal god in their practice. The tradition has been called by William Jackson as "advaitin, monistic in its outlook".The term Smarta also refers to Brahmins who specialize in the Smriti corpus of texts named the Grihya Sutras, in contrast to Shrauta Sutras. Smarta Brahmins with their focus on the Smriti corpus, contrast from Srauta Brahmins who specialize in the Sruti corpus, that is rituals and ceremonies that follow the Vedas.</t>
+          <t>Sapa'u Ruperake Petaia (born 11 April 1951) is a poet and writer from Samoa. His poem Blue Rain became the title of a collection of his poems first published in 1980 with later editions in the 1990s. The collection included the satirical poem Kidnapped (1974) which explores themes about the loss of traditional Samoan knowledge. Like other Samoan writers such as Albert Wendt, Petaia's work explores themes about the effects of colonialism and Western influences on Samoan culture and society.Petaia was born in Samoa. He attended Samoa College and worked as a clerk in the Public Service Commission in 1973. In 1978 he won a government scholarship to study at the University of the South Pacific in Fiji.</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1662,17 +1662,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Lilly Singh</t>
+          <t>Herman Mandui</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Lilly Singh (born 26 September 1988) is a Canadian YouTuber, vlogger, comedian, writer and actress. She is mostly known by her YouTube username IISuperwomanII.</t>
+          <t>Herman Mandui (1969 - October 4, 2014) was an archaeologist from Papua New Guinea.</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Lilly Singh (born September 26, 1988) is a Canadian YouTuber, comedian, talk show host, writer, and actress, who initially gained fame on social media under the pseudonym IISuperwomanII. Born and raised in Scarborough, Ontario, Singh began making YouTube videos in 2010. By 2017, she was ranked tenth on the Forbes list of the world's highest paid YouTube stars, earning a reported $10.5 million; as of September 2019 she has fourteen million subscribers and over three billion video views. Singh has featured in the annual YouTube Rewind every year since 2014 (except for 2019). Forbes named her one of the 40 most powerful people in comedy in 2019. Singh has received an MTV Fandom Award, four Streamy Awards, two Teen Choice Awards, and a People's Choice Award.</t>
+          <t>Herman Mandui (1969 – October 4, 2014) was a Papua New Guinean archaeologist. He served as the Chief Archaeologist of Papua New Guinea starting in 2008 until his death in 2014. He has been regarded as a "pioneer of archeological research" in Papua New Guinea, having worked on such sites as the Kuk Swamp in Western Highlands Province and the early human settlement sites in the Ivane Valley of the Goilala District.</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1682,17 +1682,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Pyotr Deynekin</t>
+          <t>Daniel Catan</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Pyotr Stepanovich Deynekin (14 December 1937 – 19 August 2017) was a Soviet-Russian general. He was born in Morozovsk, Russia. In 1997, he was awarded the Hero of the Russian Federation.</t>
+          <t>Daniel Catán Porteny (3 April 1949 in Mexico City - 9 April 2011 in Austin, Texas) was a Mexican opera composer of Jewish descent. He is best known for turning the Italian movie, Il Postino, into an opera. He was working at the University of Texas at Austin on a new opera based on the Frank Capra movie, Meet John Doe.</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Pyotr Stepanovich Deynekin (14 December 1937 – 19 August 2017) was a Russian military general. He was born in Morozovsk, Russia. In 1997, he was awarded the Hero of the Russian Federation.Deynekin's rank was General of the army.</t>
+          <t>Daniel Catán (April 3, 1949 – April 9, 2011) was a Mexican composer, writer and professor known particularly for his operas and his contribution of the Spanish language to the international repertory.With a compositional style described as lush, romantic and lyrical, Catán’s second opera, Rappaccini’s Daughter, became the first Mexican opera in the United States to be produced by a professional opera company.  Upon receiving international recognition, Catán’s next opera, Florencia en el Amazonas, became the first opera in Spanish to be commissioned by an opera company in the United States.  Shortly after, Catán received a Plácido Domingo Award and a Guggenheim Fellowship Award for his contributions to music.  In 2004, Catán’s opera Salsipuedes: a Tale of Love, War and Anchovies was premiered by the Houston Grand Opera.  In September 2010, his opera Il Postino was premiered by the Los Angeles Opera with Plácido Domingo singing as Pablo Neruda, a role written specifically for him.  Catán died while working on his next opera, Meet John Doe.Catán’s works also include vocal, chamber, orchestral and choral music as well as music for ballet, film and TV.</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1702,17 +1702,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Alfonso Azpiri</t>
+          <t>Blue eyed soul</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alfonso Azpiri (1947 – August 18, 2017) was a Spanish comic book artist, whose work was mainly of the adult variety. He was born in Madrid. His work has been translated and published in a number of magazines, including Heavy Metal and Penthouse Comix. </t>
+          <t>Blue Eyed Soul is a term used to describe Soul and R&amp;B music sung by white people. The term was first used in the 1960s about white artists performing music which was similar to the music being performed by Motown artists. It is sometimes called white soul.</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Alfonso Azpiri Mejía (17 January 1947 − August 18, 2017) was a Spanish comic book artist, whose work was mainly of the adult variety.</t>
+          <t>Blue-eyed soul (also known as white soul) is rhythm and blues and soul music performed by white artists.  The term was coined in the mid-1960s, to describe white artists who performed soul and R&amp;B that was similar to the music of the Motown and Stax record labels.  Though many rhythm and blues radio stations in the United States in that period would only play music by black musicians, some began to play music by white acts considered to have "soul feeling" and their music was then described as "blue-eyed soul".</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1722,17 +1722,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Duncan Russell</t>
+          <t>Monte dei Paschi di Siena</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Duncan Russell (12 March 1958 – 18 August 2017) was an English football manager. He was born in London, England. He was the manager of Conference National side Mansfield Town until 12 May 2011 when they decided not to renew his contract.Russell died in London of liver cancer on 18 August 2017 at the age of 59.</t>
+          <t>Banca Monte dei paschi di Siena (sometimes referred to as BMPS or MPS) claims to be the oldest surviving retail bank in the world. It has its headquarters in Siena, Italy.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Duncan Russell (12 March 1958 – 18 August 2017) was an English football manager who was in charge of Conference National side Mansfield Town and Hucknall Town.</t>
+          <t>Banca Monte dei Paschi di Siena S.p.A. (Italian pronunciation: [ˈbaŋka ˈmonte dei ˈpaski di ˈsjɛːna]), known as BMPS or just MPS, is an Italian bank. Tracing its history to a mount of piety founded in 1472 (548 years ago) and founded in its present form in 1624 (396 years ago), it is the world's oldest or second oldest bank, depending on the definition, and the fourth largest Italian commercial and retail bank.In 1995 the bank, then known as Monte dei Paschi di Siena, was transformed from a statutory corporation to a limited company called Banca Monte dei Paschi di Siena (Banca MPS). The Fondazione Monte dei Paschi di Siena was created to continue the charitable functions of the bank and to be, until the bailout in 2013, its largest single shareholder. Today Banca MPS has approximately 2,000 branches, 26,000 employees and 5.1 million customers in Italy, as well as branches and businesses abroad. A subsidiary, MPS Capital Services, handles corporate and investment banking.According to a research by Mediobanca and a press release by Banco BPM, Banco BPM overtook BMPS as the third largest commercial banking group in Italy in terms of total assets on 31 December 2016, after Banco BPM's formal formation on 1 January 2017. In 2016–17, BMPS was struggling to avoid a collapse, and was bailed out again by the Italian government in July 2017.</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1742,17 +1742,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Janusz Głowacki</t>
+          <t>Guebwiller</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t xml:space="preserve">Janusz Głowacki (13 September 1938 – 19 August 2017) was a Polish-American playwright, essayist and screenwriter. He was born in Poznań, Poland. </t>
+          <t>Guebwiller is a commune in the Haut-Rhin department in Grand Est of eastern France.</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Janusz Andrzej Głowacki (13 September 1938 – 19 August 2017), better known as Janusz Głowacki or colloquially simply as Głowa, was a Polish playwright, essayist and screenwriter. Głowacki was the recipient of multiple awards and honours, including Guggenheim Fellowship, two Nike Award nominations and BAFTA Award nomination. He was awarded the Gloria Artis Gold Medal in 2005 for his contribution to Polish culture, and in 2014, the Commander's Cross of the Order of Polonia Restituta.</t>
+          <t>Guebwiller (French: Guebwiller, pronounced [ɡebvilɛʁ]; Alsatian: Gàwiller [ˈkaːviləʁ]; German: Gebweiler) is a commune in the Haut-Rhin department in Grand Est currently in north-eastern France.</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -1762,17 +1762,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Sonny Burgess</t>
+          <t>Natural scientists</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Albert Austin "Sonny" Burgess (May 28, 1929 – August 18, 2017) was an American rockabilly guitarist and singer. He was born in Newport, Arkansas. He was known for working with fellow country musician D. J. Fontana. He gained popularity in Europe during most of his career. Burgess was inducted into the Rock and Roll Hall of Fame of Europe in 1999.</t>
+          <t>There are some sciences that are used to study nature. According to these sciences, the things that can be observed in nature follow certain rules. These rules are often unknown, and natural sciences are about finding them. They often use what is called the scientific method to do this.</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Albert Austin "Sonny" Burgess (May 28, 1929 – August 18, 2017) was an American rockabilly guitarist and singer.</t>
+          <t>Natural science is a branch of science concerned with the description, prediction, and understanding of natural phenomena, based on empirical evidence from observation and experimentation. Mechanisms such as peer review and repeatability of findings are used to try to ensure the validity of scientific advances.</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -1782,17 +1782,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>D. J. Fontana</t>
+          <t>Morges</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dominic Joseph "D. J." Fontana (March 15, 1931 – June 13, 2018) was an American musician. He was born in Shreveport, Louisiana. He was best known as the drummer for Elvis Presley for 14 years. He played on over 460 RCA cuts with Elvis. He also played for The Blue Moon Boys and Sonny Burgess. </t>
+          <t>Morges is a city in the Swiss canton of Vaud. It is the capital of the district Morges.</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Dominic Joseph Fontana (March 15, 1931 – June 13, 2018) was an American musician best known as the drummer for Elvis Presley for 14 years. In October 1954 he was hired to play drums for Presley, which marked the beginning of a fifteen-year relationship. He played on over 460 RCA cuts with Elvis.</t>
+          <t>Morges (Latin: Morgiis, plural, probably ablative, else dative) is a municipality in the Swiss canton of Vaud and the seat of the district of Morges. It is located on Lake Geneva.</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -1802,17 +1802,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Don Shepherd</t>
+          <t>MTS Centre</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Donald John Shepherd (12 August 1927 – 18 August 2017) was a Welsh cricketer. He played for Glamorgan. One of the great county bowlers, he took more first-class wickets, 2,218 at 21.32 each, than any other player who never played Test cricket. He was born in Port Eynon, Glamorgan, Wales. </t>
+          <t>Bell MTS Place, originally known as True North Centre and later as MTS Centre, is a sports arena in Winnipeg, Manitoba, Canada. The arena opened on November 16, 2004, and is the current home to the Winnipeg Jets of the National Hockey League (NHL). The arena was originally known as True North Centre during planning but naming rights were bought by Manitoba Telecom Services (MTS). After Bell Canada purchased MTS in spring 2017, the arena was renamed effective that May 30.The arena has been home to the Manitoba Moose of the American Hockey League (AHL), the Jets' top minor-league team, two different times. The team first played there from 2004 to 2011 before moving to St. John's, Newfoundland and Labrador, and then returned to Winnipeg in 2015.</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Donald John Shepherd (12 August 1927 – 18 August 2017) was a Welsh cricketer, who played for Glamorgan. One of the great county bowlers, he took more first-class wickets – 2,218 – than any other player who never played Test cricket.</t>
+          <t>Bell MTS Place is an indoor arena in downtown Winnipeg, Manitoba. The arena is the home of the National Hockey League's Winnipeg Jets and their American Hockey League affiliate, the Manitoba Moose.The arena stands on the former Eaton's site and is owned and operated by True North Sports &amp; Entertainment. The 440,000 square feet (41,000 m2) building was constructed at a cost of $133.5 million CAD. It opened on November 16, 2004, replacing the since-demolished Winnipeg Arena. It has a capacity of 15,321 for hockey and 16,345 for concerts.</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -1822,17 +1822,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Venero Mangano</t>
+          <t>Varna</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Venero Frank "Benny Eggs" Mangano (September 7, 1921 – August 18, 2017) was an American criminal. He was the underboss of the Genovese crime family. Since boss Daniel "Danny the Lion" Leo was imprisoned in 2007, Mangano was the family's senior leader outside prison. The nickname "Benny Eggs" came from his mother running an egg farm. He was released from prison on November 2, 2006, after serving a 15-year sentence for extortion.</t>
+          <t>Varna is a social concept from the Brahmin leaders of Hinduism in India</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Venero Frank "Benny Eggs" Mangano (September 7, 1921 – August 18, 2017) was the underboss of the Genovese crime family. Since boss Daniel "Danny the Lion" Leo was imprisoned in 2007, Mangano was the family's senior leader outside prison. The nickname "Benny Eggs" was due to an egg store his mother had run. He was released on November 2, 2006, after serving a 15-year sentence for extortion and conspiracy.</t>
+          <t>Varna (Bulgarian: Варна, pronounced [ˈvarnɐ]) is the third-largest city in Bulgaria and the largest city and seaside resort on the Bulgarian Black Sea Coast. Situated strategically in the Gulf of Varna, the city has been a major economic, social and cultural centre for almost three millennia. Varna, historically known as Odessos (Ancient Greek: Ὀδησσός), grew from a Thracian seaside settlement to a major seaport on the Black Sea.</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -1842,17 +1842,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Dominick Cirillo</t>
+          <t>Girard, Ohio</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dominick Vincent "Quiet Dom" Cirillo (born July 4, 1929) is an American gangster. He is a high-ranking member of the Genovese crime family, who briefly served as acting boss for the imprisoned Boss Vincent "Chin" Gigante. He was born in Harlem, New York. </t>
+          <t>Girard is a city in Trumbull County, Ohio, United States. The population was 9,958 at the 2010 census. It is part of Mahoning Valley.</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Dominick V. "Quiet Dom" Cirillo (born July 4, 1929 in East Harlem) is a high-ranking member of the Genovese crime family, who briefly served as acting boss for the imprisoned Boss Vincent "Chin" Gigante.</t>
+          <t>Girard is a city in Trumbull County, Ohio, United States. The population was 9,958 at the 2010 census. It is part of the Youngstown-Warren-Boardman, OH-PA Metropolitan Statistical Area.</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -1862,17 +1862,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Roger Pinto Molina</t>
+          <t>WWE World Championship</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Roger Pinto Molina (23 April 1960 – 16 August 2017) was a Bolivian right-wing politician. Pinto was born in Santa Rosa, Beni. He was elected to the Chamber of Deputies in 1997, from the single-member constituency 67 in Pando (covering areas in the provinces Nicolás Suárez, Manuripi and General Federico Román) as a Nationalist Democratic Action (ADN) candidate.</t>
+          <t>The WWE Championship is a professional wrestling world championship in WWE. It is the first world title of WWE. The title is said to be the biggest prize in professional wrestling and millions of people around the world watch matches for it.</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Roger Pinto Molina (23 April 1960 – 16 August 2017) was a Bolivian right-wing politician.</t>
+          <t>The WWE Championship is a world heavyweight championship created and promoted by the American professional wrestling promotion WWE, currently defended on their Raw brand. It is one of WWE's top three titles, alongside the Universal Championship on SmackDown and the NXT Championship on NXT. The current champion is Drew McIntyre, who is in his first reign.</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -1882,17 +1882,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Lucien N. Nedzi</t>
+          <t>Smartism</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Lucien Norbert Nedzi (born May 28, 1925) is a Democratic Party member of the United States House of Representatives from the State of Michigan.</t>
+          <t>Smartism is a sect of Hinduism in which, in contrast with Shaivism and Vaishnavism, one may worship multiple gods. It is often referred as a "liberal" sect and is passed along familial ties.</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Lucien Norbert Nedzi (born May 28, 1925) is a former Democratic member of the United States House of Representatives from the State of Michigan.  Nedzi is of Polish descent.</t>
+          <t>Smarta tradition (स्मार्त) is a movement in Hinduism that developed during its classical period around the beginning of the Common Era. It reflects a Hindu synthesis of four philosophical strands: Mimamsa, Advaita, Yoga, and theism. The Smarta tradition rejects theistic sectarianism, and it is notable for the domestic worship of five shrines with five deities, all treated as equal – Shiva, Vishnu, Surya, Ganesha, and Shakti. The Smarta tradition contrasted with the older Shrauta tradition, which was based on elaborate rituals and rites. There has been considerable overlap in the ideas and practices of the Smarta tradition with other significant historic movements within Hinduism, namely Shaivism, Brahmanism, Vaishnavism, and Shaktism.The Smarta tradition is aligned with Advaita Vedanta, and regards Adi Shankara as its founder or reformer. Shankara championed that the ultimate reality is impersonal and Nirguna (attributeless) and that any symbolic god serves the same equivalent purpose. Inspired by this belief, the Smarta tradition followers, along with the five Hindu gods include a sixth impersonal god in their practice. The tradition has been called by William Jackson as "advaitin, monistic in its outlook".The term Smarta also refers to Brahmins who specialize in the Smriti corpus of texts named the Grihya Sutras, in contrast to Shrauta Sutras. Smarta Brahmins with their focus on the Smriti corpus, contrast from Srauta Brahmins who specialize in the Sruti corpus, that is rituals and ceremonies that follow the Vedas.</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -1902,17 +1902,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Weston E. Vivian</t>
+          <t>Lilly Singh</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Weston "Wes" Edward Vivian (born October 25, 1924) is a Canadian-born American politician and retired engineer. He served as a member of the United States House of Representatives for Michigan's 2nd congressional district from January 3, 1965 through January 3, 1967. He was a member of the Democratic Party.</t>
+          <t>Lilly Singh (born 26 September 1988) is a Canadian YouTuber, vlogger, comedian, writer and actress. She is mostly known by her YouTube username IISuperwomanII.</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Weston "Wes" Edward Vivian (born October 25, 1924) is a former politician from the U.S. state of Michigan.</t>
+          <t>Lilly Singh (born September 26, 1988) is a Canadian YouTuber, comedian, talk show host, writer, and actress, who initially gained fame on social media under the pseudonym IISuperwomanII. Born and raised in Scarborough, Ontario, Singh began making YouTube videos in 2010. By 2017, she was ranked tenth on the Forbes list of the world's highest paid YouTube stars, earning a reported $10.5 million; as of September 2019 she has fourteen million subscribers and over three billion video views. Singh has featured in the annual YouTube Rewind every year since 2014 (except for 2019). Forbes named her one of the 40 most powerful people in comedy in 2019. Singh has received an MTV Fandom Award, four Streamy Awards, two Teen Choice Awards, and a People's Choice Award.</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -1922,17 +1922,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Philip Ruppe</t>
+          <t>Pyotr Deynekin</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Philip Edward Ruppe (born September 29, 1926) is an American politician. He is a member of the Republican Party. He served in the U.S. House of Representatives from 1967 to 1979 before running, unsuccessfully for the United States Senate in 1982. </t>
+          <t>Pyotr Stepanovich Deynekin (14 December 1937 – 19 August 2017) was a Soviet-Russian general. He was born in Morozovsk, Russia. In 1997, he was awarded the Hero of the Russian Federation.</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Philip Edward Ruppe (born September 29, 1926) is a former politician from the U.S. state of Michigan and a member of the Republican Party. He served in the U.S. House of Representatives from 1967 to 1979 before running, unsuccessfully for the United States Senate in 1982. He is a Korean War veteran, having served as a lieutenant in the U.S. Navy. After leaving the U.S. House, Ruppe became active in business before running for election, without success, to the 103rd Congress.</t>
+          <t>Pyotr Stepanovich Deynekin (14 December 1937 – 19 August 2017) was a Russian military general. He was born in Morozovsk, Russia. In 1997, he was awarded the Hero of the Russian Federation.Deynekin's rank was General of the army.</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -1942,17 +1942,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Dale Kildee</t>
+          <t>Alfonso Azpiri</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dale Edward Kildee (born September 16, 1929) is an American politician. He was a U.S. Representative from Michigan, serving from 1977 until 2013. He is a member of the Democratic Party. </t>
+          <t xml:space="preserve">Alfonso Azpiri (1947 – August 18, 2017) was a Spanish comic book artist, whose work was mainly of the adult variety. He was born in Madrid. His work has been translated and published in a number of magazines, including Heavy Metal and Penthouse Comix. </t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Dale Edward Kildee (born September 16, 1929) is a retired U.S. Representative from Michigan, serving from 1977 until 2013. He is a member of the Democratic Party.</t>
+          <t>Alfonso Azpiri Mejía (17 January 1947 − August 18, 2017) was a Spanish comic book artist, whose work was mainly of the adult variety.</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -1962,17 +1962,17 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Colin Meads</t>
+          <t>Duncan Russell</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Sir Colin Earl Meads (3 June 1936 – 20 August 2017) was a New Zealand rugby union player, coach and manager. He was born in Cambridge, New Zealand. He played 55 test matches (133 total games), most frequently in the lock forward position, for New Zealand's national team, the All Blacks, from 1957 until 1971.</t>
+          <t>Duncan Russell (12 March 1958 – 18 August 2017) was an English football manager. He was born in London, England. He was the manager of Conference National side Mansfield Town until 12 May 2011 when they decided not to renew his contract.Russell died in London of liver cancer on 18 August 2017 at the age of 59.</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Sir Colin Earl Meads  (3 June 1936 – 20 August 2017) was a New Zealand rugby union player. He played 55 test matches (133 games), most frequently in the lock forward position, for New Zealand's national team, the All Blacks, from 1957 until 1971.</t>
+          <t>Duncan Russell (12 March 1958 – 18 August 2017) was an English football manager who was in charge of Conference National side Mansfield Town and Hucknall Town.</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -1982,17 +1982,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Sirkka Selja</t>
+          <t>Janusz Głowacki</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Sirkka Selja (20 March 1920 – 17 August 2017) was a Finnish poet and writer. She was born in Koski Hl, nowadays Hollola, Finland. Her real name was Sirkka-Liisa Tulonen.</t>
+          <t xml:space="preserve">Janusz Głowacki (13 September 1938 – 19 August 2017) was a Polish-American playwright, essayist and screenwriter. He was born in Poznań, Poland. </t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Sirkka Selja (20 March 1920 – 17 August 2017) was a Finnish poet and writer. She was born in Hämeenkoski, Finland. Her real name was Sirkka-Liisa Tulonen.</t>
+          <t>Janusz Andrzej Głowacki (13 September 1938 – 19 August 2017), better known as Janusz Głowacki or colloquially simply as Głowa, was a Polish playwright, essayist and screenwriter. Głowacki was the recipient of multiple awards and honours, including Guggenheim Fellowship, two Nike Award nominations and BAFTA Award nomination. He was awarded the Gloria Artis Gold Medal in 2005 for his contribution to Polish culture, and in 2014, the Commander's Cross of the Order of Polonia Restituta.</t>
         </is>
       </c>
       <c r="D78" t="n">
@@ -2002,17 +2002,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>Sonny Burgess</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>April is the fourth month of the year, and comes between March and May. It is one of four months to have 30 days.</t>
+          <t>Albert Austin "Sonny" Burgess (May 28, 1929 – August 18, 2017) was an American rockabilly guitarist and singer. He was born in Newport, Arkansas. He was known for working with fellow country musician D. J. Fontana. He gained popularity in Europe during most of his career. Burgess was inducted into the Rock and Roll Hall of Fame of Europe in 1999.</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>April is the fourth month of the year in the Gregorian calendar, the fifth in the early Julian, the first of four months to have a length of 30 days, and the second of five months to have a length of less than 31 days.</t>
+          <t>Albert Austin "Sonny" Burgess (May 28, 1929 – August 18, 2017) was an American rockabilly guitarist and singer.</t>
         </is>
       </c>
       <c r="D79" t="n">
@@ -2022,17 +2022,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>D. J. Fontana</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>August (Aug.) is the eighth month of the year in the Gregorian calendar, coming between July and September. It has 31 days, the same number of days as the previous month, July, and is named after Roman Emperor Augustus Caesar.</t>
+          <t xml:space="preserve">Dominic Joseph "D. J." Fontana (March 15, 1931 – June 13, 2018) was an American musician. He was born in Shreveport, Louisiana. He was best known as the drummer for Elvis Presley for 14 years. He played on over 460 RCA cuts with Elvis. He also played for The Blue Moon Boys and Sonny Burgess. </t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>August is the eighth month of the year in the Julian and Gregorian calendars, and the fifth of seven months to have a length of 31 days. It was originally named Sextilis in Latin because it was the sixth month in the original ten-month Roman calendar under Romulus in 753 BC, with March being the first month of the year. About 700 BC, it became the eighth month when January and February were added to the year before March by King Numa Pompilius, who also gave it 29 days. Julius Caesar added two days when he created the Julian calendar in 46 BC (708 AUC), giving it its modern length of 31 days. In 8 BC, it was renamed in honor of Augustus. According to a Senatus consultum quoted by Macrobius, he chose this month because it was the time of several of his great triumphs, including the conquest of Egypt.August does not start on the same day of the week as any other month in common years, but starts on the same day of the week as February in leap years. It ends on the same day of the week as November every year. In years preceding common years, it starts and ends on the same day of the week as May of the following year. In years preceding leap years, it begins and ends on the same day of the week as October of the following year and ends on the same day of the week as February of the following year. In common years preceded by any year, August begins on the same day of the week as March and November and ends on the same day of the week as March and June. In leap years, it begins on the same day of the week as June of the previous year and ends on the same day of the week as September of the previous year. In common years preceded by common years, August begins on the same day of the week as February of the previous year.</t>
+          <t>Dominic Joseph Fontana (March 15, 1931 – June 13, 2018) was an American musician best known as the drummer for Elvis Presley for 14 years. In October 1954 he was hired to play drums for Presley, which marked the beginning of a fifteen-year relationship. He played on over 460 RCA cuts with Elvis.</t>
         </is>
       </c>
       <c r="D80" t="n">
@@ -2042,17 +2042,17 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Art</t>
+          <t>Don Shepherd</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Art is a creative activity that expresses imaginative or technical skill It produces a product, an object. Art is a diverse range of human activities in creating visual, performing artifacts, expressing the author's imaginative mind. The product of art is called a work of art, for others to experience.Some art is useful in a practical sense, such as a sculptured clay bowl that can be used. That kind of art is sometimes called a craft.</t>
+          <t xml:space="preserve">Donald John Shepherd (12 August 1927 – 18 August 2017) was a Welsh cricketer. He played for Glamorgan. One of the great county bowlers, he took more first-class wickets, 2,218 at 21.32 each, than any other player who never played Test cricket. He was born in Port Eynon, Glamorgan, Wales. </t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Art is a diverse range of human activities in creating visual, auditory or performing artifacts (artworks), expressing the author's imaginative, conceptual ideas, or technical skill, intended to be appreciated for their beauty or emotional power. Other activities related to the production of works of art include the criticism of art, the study of the history of art, and the aesthetic dissemination of art.</t>
+          <t>Donald John Shepherd (12 August 1927 – 18 August 2017) was a Welsh cricketer, who played for Glamorgan. One of the great county bowlers, he took more first-class wickets – 2,218 – than any other player who never played Test cricket.</t>
         </is>
       </c>
       <c r="D81" t="n">
@@ -2062,17 +2062,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Venero Mangano</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t xml:space="preserve">A or a is the first letter of the English alphabet. The small letter, a or α, is used as a lower case vowel.When it is spoken,  ā is said as a long a, a diphthong of ĕ and y. A is similar to  alpha of the Greek alphabet. That is not surprising, because it stands for the same sound. </t>
+          <t>Venero Frank "Benny Eggs" Mangano (September 7, 1921 – August 18, 2017) was an American criminal. He was the underboss of the Genovese crime family. Since boss Daniel "Danny the Lion" Leo was imprisoned in 2007, Mangano was the family's senior leader outside prison. The nickname "Benny Eggs" came from his mother running an egg farm. He was released from prison on November 2, 2006, after serving a 15-year sentence for extortion.</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>A or a is the first letter and the first vowel letter of the modern English alphabet and the ISO basic Latin alphabet. Its name in English is a (pronounced ), plural aes. It is similar in shape to the Ancient Greek letter alpha, from which it derives.  The uppercase version consists of the two slanting sides of a triangle, crossed in the middle by a horizontal bar. The lowercase version can be written in two forms: the double-storey a and single-storey ɑ. The latter is commonly used in handwriting and fonts based on it, especially fonts intended to be read by children, and is also found in italic type.</t>
+          <t>Venero Frank "Benny Eggs" Mangano (September 7, 1921 – August 18, 2017) was the underboss of the Genovese crime family. Since boss Daniel "Danny the Lion" Leo was imprisoned in 2007, Mangano was the family's senior leader outside prison. The nickname "Benny Eggs" was due to an egg store his mother had run. He was released on November 2, 2006, after serving a 15-year sentence for extortion and conspiracy.</t>
         </is>
       </c>
       <c r="D82" t="n">
@@ -2082,17 +2082,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Air</t>
+          <t>Dominick Cirillo</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t xml:space="preserve">Air refers to the Earth's atmosphere. Air is a mixture of many gases and dust particles. It is the clear gas in which living things live and breathe. It has an indefinite shape and volume. It has mass and weight, because it is matter. The weight of air creates atmospheric  pressure. There is no air in outer space. </t>
+          <t xml:space="preserve">Dominick Vincent "Quiet Dom" Cirillo (born July 4, 1929) is an American gangster. He is a high-ranking member of the Genovese crime family, who briefly served as acting boss for the imprisoned Boss Vincent "Chin" Gigante. He was born in Harlem, New York. </t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>The atmosphere of Earth is the layer of gases, commonly known as air, retained by Earth's gravity, surrounding the planet Earth and forming its planetary atmosphere. The atmosphere of Earth protects life on Earth by creating pressure allowing for liquid water to exist on the Earth's surface, absorbing ultraviolet solar radiation, warming the surface through heat retention (greenhouse effect), and reducing temperature extremes between day and night (the diurnal temperature variation).</t>
+          <t>Dominick V. "Quiet Dom" Cirillo (born July 4, 1929 in East Harlem) is a high-ranking member of the Genovese crime family, who briefly served as acting boss for the imprisoned Boss Vincent "Chin" Gigante.</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -2102,17 +2102,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Autonomous communities of Spain</t>
+          <t>Roger Pinto Molina</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Spain is divided in 17 parts called autonomous communities. Autonomous means that each of these autonomous communities has its own executive , legislative judicial powers. These are similar to, but not the same as, states in the United States of America, for example.</t>
+          <t>Roger Pinto Molina (23 April 1960 – 16 August 2017) was a Bolivian right-wing politician. Pinto was born in Santa Rosa, Beni. He was elected to the Chamber of Deputies in 1997, from the single-member constituency 67 in Pando (covering areas in the provinces Nicolás Suárez, Manuripi and General Federico Román) as a Nationalist Democratic Action (ADN) candidate.</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>In Spain, an autonomous community (Spanish: comunidad autónoma) is a first-level political and administrative division, created in accordance with the Spanish constitution of 1978, with the aim of guaranteeing limited autonomy of the nationalities and regions that make up Spain.Spain is not a federation, but a decentralized unitary state. While sovereignty is vested in the nation as a whole, represented in the central institutions of government, the nation has, in variable degrees, devolved power to the communities, which, in turn, exercise their right to self-government within the limits set forth in the constitution and their autonomous statutes. Each community has its own set of devolved powers; typically those communities with a stronger local nationalism have more powers; this type of devolution has been called asymmetrical. Some scholars have referred to the resulting system as a federal system in all but name, or a "federation without federalism".</t>
+          <t>Roger Pinto Molina (23 April 1960 – 16 August 2017) was a Bolivian right-wing politician.</t>
         </is>
       </c>
       <c r="D84" t="n">
@@ -2122,17 +2122,17 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Alan Turing</t>
+          <t>Lucien N. Nedzi</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Alan Mathison Turing OBE FRS (London, 23 June 1912 – Wilmslow, Cheshire, 7 June 1954) was an English mathematician and computer scientist. He was born in Maida Vale, London.</t>
+          <t>Lucien Norbert Nedzi (born May 28, 1925) is a Democratic Party member of the United States House of Representatives from the State of Michigan.</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Alan Mathison Turing  (; 23 June 1912 – 7 June 1954) was an English mathematician, computer scientist, logician, cryptanalyst, philosopher, and theoretical biologist. Turing was highly influential in the development of theoretical computer science, providing a formalisation of the concepts of algorithm and computation with the Turing machine, which can be considered a model of a general-purpose computer. Turing is widely considered to be the father of theoretical computer science and artificial intelligence. Despite these accomplishments, he was never fully recognised in his home country during his lifetime due to his homosexuality and because much of his work was covered by the Official Secrets Act.</t>
+          <t>Lucien Norbert Nedzi (born May 28, 1925) is a former Democratic member of the United States House of Representatives from the State of Michigan.  Nedzi is of Polish descent.</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -2142,17 +2142,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Alanis Morissette</t>
+          <t>Weston E. Vivian</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Alanis Nadine Morissette (born 1 June 1974) is a Grammy Award-winning Canadian-American singer and songwriter. She was born in Ottawa, Canada. She began singing in Canada as a teenager in 1990. In 1995, she became popular all over the world.</t>
+          <t>Weston "Wes" Edward Vivian (born October 25, 1924) is a Canadian-born American politician and retired engineer. He served as a member of the United States House of Representatives for Michigan's 2nd congressional district from January 3, 1965 through January 3, 1967. He was a member of the Democratic Party.</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Alanis Nadine Morissette (born June 1, 1974) is a Canadian-American singer, songwriter, record producer, and actress. Known for her emotive mezzo-soprano voice, Morissette began her career in Canada in the early 1990s with two mildly successful dance-pop albums. Afterwards, as part of a recording deal, she moved to Holmby Hills, Los Angeles and in 1995 released Jagged Little Pill, a more rock-oriented album which sold more than 33 million copies globally and is her most critically acclaimed work. Her follow-up album, Supposed Former Infatuation Junkie, was released in 1998.</t>
+          <t>Weston "Wes" Edward Vivian (born October 25, 1924) is a former politician from the U.S. state of Michigan.</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -2162,17 +2162,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Adobe Illustrator</t>
+          <t>Philip Ruppe</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Adobe Illustrator is a computer program for making graphic design and illustrations. It is made by Adobe Systems. Pictures created in Adobe Illustrator can be made bigger or smaller, and look exactly the same at any size. It works well with the rest of the products with the Adobe name.</t>
+          <t xml:space="preserve">Philip Edward Ruppe (born September 29, 1926) is an American politician. He is a member of the Republican Party. He served in the U.S. House of Representatives from 1967 to 1979 before running, unsuccessfully for the United States Senate in 1982. </t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Adobe Illustrator is a vector graphics editor developed and marketed by Adobe Inc. Originally designed for the Apple Macintosh, development of Adobe Illustrator began in 1985. Along with Creative Cloud (Adobe's shift to monthly or annual subscription service delivered over the Internet), Illustrator CC was released. The latest version, Illustrator CC 2020, was released on October 24, 2019 and is the 24th generation in the product line. Adobe Illustrator was reviewed as the best vector graphics editing program in 2018 by PC Magazine.</t>
+          <t>Philip Edward Ruppe (born September 29, 1926) is a former politician from the U.S. state of Michigan and a member of the Republican Party. He served in the U.S. House of Representatives from 1967 to 1979 before running, unsuccessfully for the United States Senate in 1982. He is a Korean War veteran, having served as a lieutenant in the U.S. Navy. After leaving the U.S. House, Ruppe became active in business before running for election, without success, to the 103rd Congress.</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2182,23 +2182,64 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Andouille</t>
+          <t>Dale Kildee</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Andouille is a type of pork sausage. It is spicy (hot in taste) and smoked. There are different kinds, all with different combinations of pork meat, fat, intestines (tubes going to the stomach), and tripe (the wall of the stomach). Andouille sausage first came from France or Germany (no-one is sure), but the name indicates that it may have come out from France, and the most famous sort in the USA is the "Cajun" style. </t>
+          <t xml:space="preserve">Dale Edward Kildee (born September 16, 1929) is an American politician. He was a U.S. Representative from Michigan, serving from 1977 until 2013. He is a member of the Democratic Party. </t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Andouille (US:  ann-DOO-ee; French: [ɑ̃duj]; from Vulgar Latin verb inducere, meaning "to lead in") is a smoked sausage made using pork, originating in France.</t>
+          <t>Dale Edward Kildee (born September 16, 1929) is a retired U.S. Representative from Michigan, serving from 1977 until 2013. He is a member of the Democratic Party.</t>
         </is>
       </c>
       <c r="D88" t="n">
         <v>86</v>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Colin Meads</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Sir Colin Earl Meads (3 June 1936 – 20 August 2017) was a New Zealand rugby union player, coach and manager. He was born in Cambridge, New Zealand. He played 55 test matches (133 total games), most frequently in the lock forward position, for New Zealand's national team, the All Blacks, from 1957 until 1971.</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Sir Colin Earl Meads  (3 June 1936 – 20 August 2017) was a New Zealand rugby union player. He played 55 test matches (133 games), most frequently in the lock forward position, for New Zealand's national team, the All Blacks, from 1957 until 1971.</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Sirkka Selja</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Sirkka Selja (20 March 1920 – 17 August 2017) was a Finnish poet and writer. She was born in Koski Hl, nowadays Hollola, Finland. Her real name was Sirkka-Liisa Tulonen.</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Sirkka Selja (20 March 1920 – 17 August 2017) was a Finnish poet and writer. She was born in Hämeenkoski, Finland. Her real name was Sirkka-Liisa Tulonen.</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>